<commit_message>
updated DBs and sort of handle duplicate clozes
</commit_message>
<xml_diff>
--- a/Databases/中文_sentences.xlsx
+++ b/Databases/中文_sentences.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="544" uniqueCount="302">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="647" uniqueCount="363">
   <si>
     <t>FOREIGN</t>
   </si>
@@ -397,6 +397,81 @@
     <t xml:space="preserve">他想用讽刺来激怒我们。  </t>
   </si>
   <si>
+    <t xml:space="preserve">存在即被感知。  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">我打个电话即到。  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">康熙一继位即命人修史。  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">这个化学反应产生很多热量。  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">气体之间通过热对流传导热量。  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">热力学定律解释了热量转化的原理。  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">要想身体健康，就要多注意饮食营养配比。  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">生石灰配比  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">贵金属配比  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">桌子摆放得很起眼儿。  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">茶几摆放得非常合适。  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">这些家具都毫无用处地摆放着。  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">他们肯定要摄入大量的水份。  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">在健康状态下，液体的摄入与排出应是均衡的。  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">表4是一个典型的一天食物摄入的范例。  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">腹鳍对应着四足动物的后肢。  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">蝙蝠的翅膀和人的胳膊是对应的。  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">我们可以发现这些抗体是特定对应每种蛋白质的。  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">除此以外  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">好除此以外  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">除此以外，看不出还有什么别的原因会使她与达切发生一段短暂的、充满不安的恋情。  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">利益逐渐消失。  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">风逐渐停了。  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">利润逐渐下滑。  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">习惯是后天养成的。  </t>
+  </si>
+  <si>
     <t>I didn't even mind the lack of an in-flight meal service.</t>
   </si>
   <si>
@@ -766,6 +841,84 @@
     <t>He aims to offend us with his satire.</t>
   </si>
   <si>
+    <t>Being is being perceived.</t>
+  </si>
+  <si>
+    <t>I will be there immediately – I just have to make a phone call.</t>
+  </si>
+  <si>
+    <t>Kang Xi ordered people to compile historical books the moment he succeeded to the throne.</t>
+  </si>
+  <si>
+    <t>This chemical reaction generates a lot of heat.</t>
+  </si>
+  <si>
+    <t>Gases transmit heat through thermal convention.</t>
+  </si>
+  <si>
+    <t>The Law of Thermodynamics explains the transfer of heat.</t>
+  </si>
+  <si>
+    <t>Pay attention to the amount of nutrition in your food if you want to be healthy.</t>
+  </si>
+  <si>
+    <t>lime proportion.</t>
+  </si>
+  <si>
+    <t>Precious metals ratio.</t>
+  </si>
+  <si>
+    <t>The table was set appealingly.</t>
+  </si>
+  <si>
+    <t>End tables placed conveniently.</t>
+  </si>
+  <si>
+    <t>The furniture was sitting around uselessly.</t>
+  </si>
+  <si>
+    <t>They will certainly need to take in plenty of liquid.</t>
+  </si>
+  <si>
+    <t>In health，fluid intake is usually balanced with output.</t>
+  </si>
+  <si>
+    <t>Table 4 is an example of a typical day's food intake.</t>
+  </si>
+  <si>
+    <t>Ventral (or pelvic) fins correspond to the hind limbs of a quadruped.</t>
+  </si>
+  <si>
+    <t>The wing of a bat and the arm of a man are homologous.</t>
+  </si>
+  <si>
+    <t>We were able to see that these antibodies are specific to each protein.</t>
+  </si>
+  <si>
+    <t>Put that aside.</t>
+  </si>
+  <si>
+    <t>Yes, put that aside.</t>
+  </si>
+  <si>
+    <t>No other explanation is offered for her decision to enter into a brief, nervous affair with Dutch.</t>
+  </si>
+  <si>
+    <t>Interest tapered off.</t>
+  </si>
+  <si>
+    <t>The wind gradually died away.</t>
+  </si>
+  <si>
+    <t>The interest declined by little and little.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Xíguàn shìhòutiān yǎng chéng de. </t>
+  </si>
+  <si>
+    <t>Yǎngchéng jiàoyù hěn zhòngyào，yào zhùyì péiyǎng háizi de liánghǎo xíguàn.</t>
+  </si>
+  <si>
     <t>餐饮</t>
   </si>
   <si>
@@ -907,6 +1060,33 @@
     <t>讽刺</t>
   </si>
   <si>
+    <t>即</t>
+  </si>
+  <si>
+    <t>热量</t>
+  </si>
+  <si>
+    <t>配比</t>
+  </si>
+  <si>
+    <t>摆放</t>
+  </si>
+  <si>
+    <t>摄入</t>
+  </si>
+  <si>
+    <t>对应</t>
+  </si>
+  <si>
+    <t>除此以外</t>
+  </si>
+  <si>
+    <t>逐渐</t>
+  </si>
+  <si>
+    <t>养成</t>
+  </si>
+  <si>
     <t>2020-11-25</t>
   </si>
   <si>
@@ -920,6 +1100,9 @@
   </si>
   <si>
     <t>2020-11-30</t>
+  </si>
+  <si>
+    <t>2020-12-02</t>
   </si>
 </sst>
 </file>
@@ -1277,7 +1460,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D136"/>
+  <dimension ref="A1:D162"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1302,13 +1485,13 @@
         <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>127</v>
+        <v>152</v>
       </c>
       <c r="C2" t="s">
-        <v>250</v>
+        <v>301</v>
       </c>
       <c r="D2" t="s">
-        <v>297</v>
+        <v>357</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -1316,13 +1499,13 @@
         <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>128</v>
+        <v>153</v>
       </c>
       <c r="C3" t="s">
-        <v>250</v>
+        <v>301</v>
       </c>
       <c r="D3" t="s">
-        <v>297</v>
+        <v>357</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -1330,13 +1513,13 @@
         <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>129</v>
+        <v>154</v>
       </c>
       <c r="C4" t="s">
-        <v>250</v>
+        <v>301</v>
       </c>
       <c r="D4" t="s">
-        <v>297</v>
+        <v>357</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -1344,13 +1527,13 @@
         <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>130</v>
+        <v>155</v>
       </c>
       <c r="C5" t="s">
-        <v>251</v>
+        <v>302</v>
       </c>
       <c r="D5" t="s">
-        <v>297</v>
+        <v>357</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -1358,13 +1541,13 @@
         <v>8</v>
       </c>
       <c r="B6" t="s">
-        <v>131</v>
+        <v>156</v>
       </c>
       <c r="C6" t="s">
-        <v>251</v>
+        <v>302</v>
       </c>
       <c r="D6" t="s">
-        <v>297</v>
+        <v>357</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -1372,13 +1555,13 @@
         <v>9</v>
       </c>
       <c r="B7" t="s">
-        <v>132</v>
+        <v>157</v>
       </c>
       <c r="C7" t="s">
-        <v>251</v>
+        <v>302</v>
       </c>
       <c r="D7" t="s">
-        <v>297</v>
+        <v>357</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -1386,13 +1569,13 @@
         <v>10</v>
       </c>
       <c r="B8" t="s">
-        <v>133</v>
+        <v>158</v>
       </c>
       <c r="C8" t="s">
-        <v>252</v>
+        <v>303</v>
       </c>
       <c r="D8" t="s">
-        <v>297</v>
+        <v>357</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -1400,13 +1583,13 @@
         <v>11</v>
       </c>
       <c r="B9" t="s">
-        <v>134</v>
+        <v>159</v>
       </c>
       <c r="C9" t="s">
-        <v>252</v>
+        <v>303</v>
       </c>
       <c r="D9" t="s">
-        <v>297</v>
+        <v>357</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -1414,13 +1597,13 @@
         <v>12</v>
       </c>
       <c r="B10" t="s">
-        <v>135</v>
+        <v>160</v>
       </c>
       <c r="C10" t="s">
-        <v>252</v>
+        <v>303</v>
       </c>
       <c r="D10" t="s">
-        <v>297</v>
+        <v>357</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -1428,13 +1611,13 @@
         <v>13</v>
       </c>
       <c r="B11" t="s">
-        <v>136</v>
+        <v>161</v>
       </c>
       <c r="C11" t="s">
-        <v>253</v>
+        <v>304</v>
       </c>
       <c r="D11" t="s">
-        <v>297</v>
+        <v>357</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -1442,13 +1625,13 @@
         <v>14</v>
       </c>
       <c r="B12" t="s">
-        <v>137</v>
+        <v>162</v>
       </c>
       <c r="C12" t="s">
-        <v>253</v>
+        <v>304</v>
       </c>
       <c r="D12" t="s">
-        <v>297</v>
+        <v>357</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -1456,13 +1639,13 @@
         <v>15</v>
       </c>
       <c r="B13" t="s">
-        <v>138</v>
+        <v>163</v>
       </c>
       <c r="C13" t="s">
-        <v>253</v>
+        <v>304</v>
       </c>
       <c r="D13" t="s">
-        <v>297</v>
+        <v>357</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -1470,13 +1653,13 @@
         <v>16</v>
       </c>
       <c r="B14" t="s">
-        <v>139</v>
+        <v>164</v>
       </c>
       <c r="C14" t="s">
-        <v>254</v>
+        <v>305</v>
       </c>
       <c r="D14" t="s">
-        <v>297</v>
+        <v>357</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -1484,13 +1667,13 @@
         <v>17</v>
       </c>
       <c r="B15" t="s">
-        <v>140</v>
+        <v>165</v>
       </c>
       <c r="C15" t="s">
-        <v>254</v>
+        <v>305</v>
       </c>
       <c r="D15" t="s">
-        <v>297</v>
+        <v>357</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -1498,13 +1681,13 @@
         <v>18</v>
       </c>
       <c r="B16" t="s">
-        <v>141</v>
+        <v>166</v>
       </c>
       <c r="C16" t="s">
-        <v>254</v>
+        <v>305</v>
       </c>
       <c r="D16" t="s">
-        <v>297</v>
+        <v>357</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -1512,13 +1695,13 @@
         <v>19</v>
       </c>
       <c r="B17" t="s">
-        <v>142</v>
+        <v>167</v>
       </c>
       <c r="C17" t="s">
-        <v>255</v>
+        <v>306</v>
       </c>
       <c r="D17" t="s">
-        <v>297</v>
+        <v>357</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -1526,13 +1709,13 @@
         <v>20</v>
       </c>
       <c r="B18" t="s">
-        <v>143</v>
+        <v>168</v>
       </c>
       <c r="C18" t="s">
-        <v>255</v>
+        <v>306</v>
       </c>
       <c r="D18" t="s">
-        <v>297</v>
+        <v>357</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -1540,13 +1723,13 @@
         <v>21</v>
       </c>
       <c r="B19" t="s">
-        <v>144</v>
+        <v>169</v>
       </c>
       <c r="C19" t="s">
-        <v>255</v>
+        <v>306</v>
       </c>
       <c r="D19" t="s">
-        <v>297</v>
+        <v>357</v>
       </c>
     </row>
     <row r="20" spans="1:4">
@@ -1554,13 +1737,13 @@
         <v>22</v>
       </c>
       <c r="B20" t="s">
-        <v>145</v>
+        <v>170</v>
       </c>
       <c r="C20" t="s">
-        <v>256</v>
+        <v>307</v>
       </c>
       <c r="D20" t="s">
-        <v>297</v>
+        <v>357</v>
       </c>
     </row>
     <row r="21" spans="1:4">
@@ -1568,13 +1751,13 @@
         <v>23</v>
       </c>
       <c r="B21" t="s">
-        <v>146</v>
+        <v>171</v>
       </c>
       <c r="C21" t="s">
-        <v>256</v>
+        <v>307</v>
       </c>
       <c r="D21" t="s">
-        <v>297</v>
+        <v>357</v>
       </c>
     </row>
     <row r="22" spans="1:4">
@@ -1582,13 +1765,13 @@
         <v>24</v>
       </c>
       <c r="B22" t="s">
-        <v>147</v>
+        <v>172</v>
       </c>
       <c r="C22" t="s">
-        <v>256</v>
+        <v>307</v>
       </c>
       <c r="D22" t="s">
-        <v>297</v>
+        <v>357</v>
       </c>
     </row>
     <row r="23" spans="1:4">
@@ -1596,13 +1779,13 @@
         <v>25</v>
       </c>
       <c r="B23" t="s">
-        <v>148</v>
+        <v>173</v>
       </c>
       <c r="C23" t="s">
-        <v>257</v>
+        <v>308</v>
       </c>
       <c r="D23" t="s">
-        <v>297</v>
+        <v>357</v>
       </c>
     </row>
     <row r="24" spans="1:4">
@@ -1610,13 +1793,13 @@
         <v>26</v>
       </c>
       <c r="B24" t="s">
-        <v>149</v>
+        <v>174</v>
       </c>
       <c r="C24" t="s">
-        <v>257</v>
+        <v>308</v>
       </c>
       <c r="D24" t="s">
-        <v>297</v>
+        <v>357</v>
       </c>
     </row>
     <row r="25" spans="1:4">
@@ -1624,13 +1807,13 @@
         <v>27</v>
       </c>
       <c r="B25" t="s">
-        <v>150</v>
+        <v>175</v>
       </c>
       <c r="C25" t="s">
-        <v>257</v>
+        <v>308</v>
       </c>
       <c r="D25" t="s">
-        <v>297</v>
+        <v>357</v>
       </c>
     </row>
     <row r="26" spans="1:4">
@@ -1638,13 +1821,13 @@
         <v>28</v>
       </c>
       <c r="B26" t="s">
-        <v>151</v>
+        <v>176</v>
       </c>
       <c r="C26" t="s">
-        <v>258</v>
+        <v>309</v>
       </c>
       <c r="D26" t="s">
-        <v>297</v>
+        <v>357</v>
       </c>
     </row>
     <row r="27" spans="1:4">
@@ -1652,13 +1835,13 @@
         <v>29</v>
       </c>
       <c r="B27" t="s">
-        <v>152</v>
+        <v>177</v>
       </c>
       <c r="C27" t="s">
-        <v>258</v>
+        <v>309</v>
       </c>
       <c r="D27" t="s">
-        <v>297</v>
+        <v>357</v>
       </c>
     </row>
     <row r="28" spans="1:4">
@@ -1666,13 +1849,13 @@
         <v>30</v>
       </c>
       <c r="B28" t="s">
-        <v>153</v>
+        <v>178</v>
       </c>
       <c r="C28" t="s">
-        <v>258</v>
+        <v>309</v>
       </c>
       <c r="D28" t="s">
-        <v>297</v>
+        <v>357</v>
       </c>
     </row>
     <row r="29" spans="1:4">
@@ -1680,13 +1863,13 @@
         <v>31</v>
       </c>
       <c r="B29" t="s">
-        <v>154</v>
+        <v>179</v>
       </c>
       <c r="C29" t="s">
-        <v>259</v>
+        <v>310</v>
       </c>
       <c r="D29" t="s">
-        <v>298</v>
+        <v>358</v>
       </c>
     </row>
     <row r="30" spans="1:4">
@@ -1694,13 +1877,13 @@
         <v>32</v>
       </c>
       <c r="B30" t="s">
-        <v>155</v>
+        <v>180</v>
       </c>
       <c r="C30" t="s">
-        <v>259</v>
+        <v>310</v>
       </c>
       <c r="D30" t="s">
-        <v>298</v>
+        <v>358</v>
       </c>
     </row>
     <row r="31" spans="1:4">
@@ -1708,13 +1891,13 @@
         <v>33</v>
       </c>
       <c r="B31" t="s">
-        <v>156</v>
+        <v>181</v>
       </c>
       <c r="C31" t="s">
-        <v>259</v>
+        <v>310</v>
       </c>
       <c r="D31" t="s">
-        <v>298</v>
+        <v>358</v>
       </c>
     </row>
     <row r="32" spans="1:4">
@@ -1722,13 +1905,13 @@
         <v>34</v>
       </c>
       <c r="B32" t="s">
-        <v>157</v>
+        <v>182</v>
       </c>
       <c r="C32" t="s">
-        <v>260</v>
+        <v>311</v>
       </c>
       <c r="D32" t="s">
-        <v>298</v>
+        <v>358</v>
       </c>
     </row>
     <row r="33" spans="1:4">
@@ -1736,13 +1919,13 @@
         <v>35</v>
       </c>
       <c r="B33" t="s">
-        <v>158</v>
+        <v>183</v>
       </c>
       <c r="C33" t="s">
-        <v>260</v>
+        <v>311</v>
       </c>
       <c r="D33" t="s">
-        <v>298</v>
+        <v>358</v>
       </c>
     </row>
     <row r="34" spans="1:4">
@@ -1750,13 +1933,13 @@
         <v>36</v>
       </c>
       <c r="B34" t="s">
-        <v>159</v>
+        <v>184</v>
       </c>
       <c r="C34" t="s">
-        <v>260</v>
+        <v>311</v>
       </c>
       <c r="D34" t="s">
-        <v>298</v>
+        <v>358</v>
       </c>
     </row>
     <row r="35" spans="1:4">
@@ -1764,13 +1947,13 @@
         <v>37</v>
       </c>
       <c r="B35" t="s">
-        <v>160</v>
+        <v>185</v>
       </c>
       <c r="C35" t="s">
-        <v>261</v>
+        <v>312</v>
       </c>
       <c r="D35" t="s">
-        <v>298</v>
+        <v>358</v>
       </c>
     </row>
     <row r="36" spans="1:4">
@@ -1778,13 +1961,13 @@
         <v>38</v>
       </c>
       <c r="B36" t="s">
-        <v>161</v>
+        <v>186</v>
       </c>
       <c r="C36" t="s">
-        <v>261</v>
+        <v>312</v>
       </c>
       <c r="D36" t="s">
-        <v>298</v>
+        <v>358</v>
       </c>
     </row>
     <row r="37" spans="1:4">
@@ -1792,13 +1975,13 @@
         <v>5</v>
       </c>
       <c r="B37" t="s">
-        <v>128</v>
+        <v>153</v>
       </c>
       <c r="C37" t="s">
-        <v>261</v>
+        <v>312</v>
       </c>
       <c r="D37" t="s">
-        <v>298</v>
+        <v>358</v>
       </c>
     </row>
     <row r="38" spans="1:4">
@@ -1806,13 +1989,13 @@
         <v>39</v>
       </c>
       <c r="B38" t="s">
-        <v>162</v>
+        <v>187</v>
       </c>
       <c r="C38" t="s">
-        <v>262</v>
+        <v>313</v>
       </c>
       <c r="D38" t="s">
-        <v>298</v>
+        <v>358</v>
       </c>
     </row>
     <row r="39" spans="1:4">
@@ -1820,13 +2003,13 @@
         <v>40</v>
       </c>
       <c r="B39" t="s">
-        <v>163</v>
+        <v>188</v>
       </c>
       <c r="C39" t="s">
-        <v>262</v>
+        <v>313</v>
       </c>
       <c r="D39" t="s">
-        <v>298</v>
+        <v>358</v>
       </c>
     </row>
     <row r="40" spans="1:4">
@@ -1834,13 +2017,13 @@
         <v>41</v>
       </c>
       <c r="B40" t="s">
-        <v>164</v>
+        <v>189</v>
       </c>
       <c r="C40" t="s">
-        <v>262</v>
+        <v>313</v>
       </c>
       <c r="D40" t="s">
-        <v>298</v>
+        <v>358</v>
       </c>
     </row>
     <row r="41" spans="1:4">
@@ -1848,13 +2031,13 @@
         <v>42</v>
       </c>
       <c r="B41" t="s">
-        <v>165</v>
+        <v>190</v>
       </c>
       <c r="C41" t="s">
-        <v>263</v>
+        <v>314</v>
       </c>
       <c r="D41" t="s">
-        <v>298</v>
+        <v>358</v>
       </c>
     </row>
     <row r="42" spans="1:4">
@@ -1862,13 +2045,13 @@
         <v>43</v>
       </c>
       <c r="B42" t="s">
-        <v>166</v>
+        <v>191</v>
       </c>
       <c r="C42" t="s">
-        <v>263</v>
+        <v>314</v>
       </c>
       <c r="D42" t="s">
-        <v>298</v>
+        <v>358</v>
       </c>
     </row>
     <row r="43" spans="1:4">
@@ -1876,13 +2059,13 @@
         <v>44</v>
       </c>
       <c r="B43" t="s">
-        <v>167</v>
+        <v>192</v>
       </c>
       <c r="C43" t="s">
-        <v>263</v>
+        <v>314</v>
       </c>
       <c r="D43" t="s">
-        <v>298</v>
+        <v>358</v>
       </c>
     </row>
     <row r="44" spans="1:4">
@@ -1890,13 +2073,13 @@
         <v>45</v>
       </c>
       <c r="B44" t="s">
-        <v>168</v>
+        <v>193</v>
       </c>
       <c r="C44" t="s">
-        <v>264</v>
+        <v>315</v>
       </c>
       <c r="D44" t="s">
-        <v>298</v>
+        <v>358</v>
       </c>
     </row>
     <row r="45" spans="1:4">
@@ -1904,13 +2087,13 @@
         <v>46</v>
       </c>
       <c r="B45" t="s">
-        <v>169</v>
+        <v>194</v>
       </c>
       <c r="C45" t="s">
-        <v>264</v>
+        <v>315</v>
       </c>
       <c r="D45" t="s">
-        <v>298</v>
+        <v>358</v>
       </c>
     </row>
     <row r="46" spans="1:4">
@@ -1918,13 +2101,13 @@
         <v>47</v>
       </c>
       <c r="B46" t="s">
-        <v>170</v>
+        <v>195</v>
       </c>
       <c r="C46" t="s">
-        <v>264</v>
+        <v>315</v>
       </c>
       <c r="D46" t="s">
-        <v>298</v>
+        <v>358</v>
       </c>
     </row>
     <row r="47" spans="1:4">
@@ -1932,13 +2115,13 @@
         <v>48</v>
       </c>
       <c r="B47" t="s">
-        <v>171</v>
+        <v>196</v>
       </c>
       <c r="C47" t="s">
-        <v>265</v>
+        <v>316</v>
       </c>
       <c r="D47" t="s">
-        <v>298</v>
+        <v>358</v>
       </c>
     </row>
     <row r="48" spans="1:4">
@@ -1946,13 +2129,13 @@
         <v>49</v>
       </c>
       <c r="B48" t="s">
-        <v>172</v>
+        <v>197</v>
       </c>
       <c r="C48" t="s">
-        <v>265</v>
+        <v>316</v>
       </c>
       <c r="D48" t="s">
-        <v>298</v>
+        <v>358</v>
       </c>
     </row>
     <row r="49" spans="1:4">
@@ -1960,13 +2143,13 @@
         <v>50</v>
       </c>
       <c r="B49" t="s">
-        <v>173</v>
+        <v>198</v>
       </c>
       <c r="C49" t="s">
-        <v>265</v>
+        <v>316</v>
       </c>
       <c r="D49" t="s">
-        <v>298</v>
+        <v>358</v>
       </c>
     </row>
     <row r="50" spans="1:4">
@@ -1974,13 +2157,13 @@
         <v>51</v>
       </c>
       <c r="B50" t="s">
-        <v>174</v>
+        <v>199</v>
       </c>
       <c r="C50" t="s">
-        <v>266</v>
+        <v>317</v>
       </c>
       <c r="D50" t="s">
-        <v>298</v>
+        <v>358</v>
       </c>
     </row>
     <row r="51" spans="1:4">
@@ -1988,13 +2171,13 @@
         <v>52</v>
       </c>
       <c r="B51" t="s">
-        <v>175</v>
+        <v>200</v>
       </c>
       <c r="C51" t="s">
-        <v>267</v>
+        <v>318</v>
       </c>
       <c r="D51" t="s">
-        <v>298</v>
+        <v>358</v>
       </c>
     </row>
     <row r="52" spans="1:4">
@@ -2002,13 +2185,13 @@
         <v>53</v>
       </c>
       <c r="B52" t="s">
-        <v>176</v>
+        <v>201</v>
       </c>
       <c r="C52" t="s">
-        <v>267</v>
+        <v>318</v>
       </c>
       <c r="D52" t="s">
-        <v>298</v>
+        <v>358</v>
       </c>
     </row>
     <row r="53" spans="1:4">
@@ -2016,13 +2199,13 @@
         <v>54</v>
       </c>
       <c r="B53" t="s">
-        <v>177</v>
+        <v>202</v>
       </c>
       <c r="C53" t="s">
-        <v>267</v>
+        <v>318</v>
       </c>
       <c r="D53" t="s">
-        <v>298</v>
+        <v>358</v>
       </c>
     </row>
     <row r="54" spans="1:4">
@@ -2030,13 +2213,13 @@
         <v>55</v>
       </c>
       <c r="B54" t="s">
-        <v>178</v>
+        <v>203</v>
       </c>
       <c r="C54" t="s">
-        <v>268</v>
+        <v>319</v>
       </c>
       <c r="D54" t="s">
-        <v>298</v>
+        <v>358</v>
       </c>
     </row>
     <row r="55" spans="1:4">
@@ -2044,13 +2227,13 @@
         <v>56</v>
       </c>
       <c r="B55" t="s">
-        <v>179</v>
+        <v>204</v>
       </c>
       <c r="C55" t="s">
-        <v>268</v>
+        <v>319</v>
       </c>
       <c r="D55" t="s">
-        <v>298</v>
+        <v>358</v>
       </c>
     </row>
     <row r="56" spans="1:4">
@@ -2058,13 +2241,13 @@
         <v>57</v>
       </c>
       <c r="B56" t="s">
-        <v>180</v>
+        <v>205</v>
       </c>
       <c r="C56" t="s">
-        <v>268</v>
+        <v>319</v>
       </c>
       <c r="D56" t="s">
-        <v>298</v>
+        <v>358</v>
       </c>
     </row>
     <row r="57" spans="1:4">
@@ -2072,13 +2255,13 @@
         <v>58</v>
       </c>
       <c r="B57" t="s">
-        <v>181</v>
+        <v>206</v>
       </c>
       <c r="C57" t="s">
-        <v>269</v>
+        <v>320</v>
       </c>
       <c r="D57" t="s">
-        <v>298</v>
+        <v>358</v>
       </c>
     </row>
     <row r="58" spans="1:4">
@@ -2086,13 +2269,13 @@
         <v>59</v>
       </c>
       <c r="B58" t="s">
-        <v>182</v>
+        <v>207</v>
       </c>
       <c r="C58" t="s">
-        <v>270</v>
+        <v>321</v>
       </c>
       <c r="D58" t="s">
-        <v>298</v>
+        <v>358</v>
       </c>
     </row>
     <row r="59" spans="1:4">
@@ -2100,13 +2283,13 @@
         <v>60</v>
       </c>
       <c r="B59" t="s">
-        <v>183</v>
+        <v>208</v>
       </c>
       <c r="C59" t="s">
-        <v>270</v>
+        <v>321</v>
       </c>
       <c r="D59" t="s">
-        <v>298</v>
+        <v>358</v>
       </c>
     </row>
     <row r="60" spans="1:4">
@@ -2114,13 +2297,13 @@
         <v>61</v>
       </c>
       <c r="B60" t="s">
-        <v>184</v>
+        <v>209</v>
       </c>
       <c r="C60" t="s">
-        <v>270</v>
+        <v>321</v>
       </c>
       <c r="D60" t="s">
-        <v>298</v>
+        <v>358</v>
       </c>
     </row>
     <row r="61" spans="1:4">
@@ -2128,13 +2311,13 @@
         <v>62</v>
       </c>
       <c r="B61" t="s">
-        <v>185</v>
+        <v>210</v>
       </c>
       <c r="C61" t="s">
-        <v>271</v>
+        <v>322</v>
       </c>
       <c r="D61" t="s">
-        <v>298</v>
+        <v>358</v>
       </c>
     </row>
     <row r="62" spans="1:4">
@@ -2142,13 +2325,13 @@
         <v>63</v>
       </c>
       <c r="B62" t="s">
-        <v>186</v>
+        <v>211</v>
       </c>
       <c r="C62" t="s">
-        <v>271</v>
+        <v>322</v>
       </c>
       <c r="D62" t="s">
-        <v>298</v>
+        <v>358</v>
       </c>
     </row>
     <row r="63" spans="1:4">
@@ -2156,13 +2339,13 @@
         <v>64</v>
       </c>
       <c r="B63" t="s">
-        <v>187</v>
+        <v>212</v>
       </c>
       <c r="C63" t="s">
-        <v>271</v>
+        <v>322</v>
       </c>
       <c r="D63" t="s">
-        <v>298</v>
+        <v>358</v>
       </c>
     </row>
     <row r="64" spans="1:4">
@@ -2170,13 +2353,13 @@
         <v>65</v>
       </c>
       <c r="B64" t="s">
-        <v>188</v>
+        <v>213</v>
       </c>
       <c r="C64" t="s">
-        <v>272</v>
+        <v>323</v>
       </c>
       <c r="D64" t="s">
-        <v>298</v>
+        <v>358</v>
       </c>
     </row>
     <row r="65" spans="1:4">
@@ -2184,13 +2367,13 @@
         <v>66</v>
       </c>
       <c r="B65" t="s">
-        <v>189</v>
+        <v>214</v>
       </c>
       <c r="C65" t="s">
-        <v>272</v>
+        <v>323</v>
       </c>
       <c r="D65" t="s">
-        <v>298</v>
+        <v>358</v>
       </c>
     </row>
     <row r="66" spans="1:4">
@@ -2198,13 +2381,13 @@
         <v>67</v>
       </c>
       <c r="B66" t="s">
-        <v>190</v>
+        <v>215</v>
       </c>
       <c r="C66" t="s">
-        <v>272</v>
+        <v>323</v>
       </c>
       <c r="D66" t="s">
-        <v>298</v>
+        <v>358</v>
       </c>
     </row>
     <row r="67" spans="1:4">
@@ -2212,13 +2395,13 @@
         <v>68</v>
       </c>
       <c r="B67" t="s">
-        <v>191</v>
+        <v>216</v>
       </c>
       <c r="C67" t="s">
-        <v>273</v>
+        <v>324</v>
       </c>
       <c r="D67" t="s">
-        <v>298</v>
+        <v>358</v>
       </c>
     </row>
     <row r="68" spans="1:4">
@@ -2226,13 +2409,13 @@
         <v>69</v>
       </c>
       <c r="B68" t="s">
-        <v>192</v>
+        <v>217</v>
       </c>
       <c r="C68" t="s">
-        <v>273</v>
+        <v>324</v>
       </c>
       <c r="D68" t="s">
-        <v>298</v>
+        <v>358</v>
       </c>
     </row>
     <row r="69" spans="1:4">
@@ -2240,13 +2423,13 @@
         <v>70</v>
       </c>
       <c r="B69" t="s">
-        <v>193</v>
+        <v>218</v>
       </c>
       <c r="C69" t="s">
-        <v>273</v>
+        <v>324</v>
       </c>
       <c r="D69" t="s">
-        <v>298</v>
+        <v>358</v>
       </c>
     </row>
     <row r="70" spans="1:4">
@@ -2254,13 +2437,13 @@
         <v>71</v>
       </c>
       <c r="B70" t="s">
-        <v>194</v>
+        <v>219</v>
       </c>
       <c r="C70" t="s">
-        <v>274</v>
+        <v>325</v>
       </c>
       <c r="D70" t="s">
-        <v>299</v>
+        <v>359</v>
       </c>
     </row>
     <row r="71" spans="1:4">
@@ -2268,13 +2451,13 @@
         <v>72</v>
       </c>
       <c r="B71" t="s">
-        <v>195</v>
+        <v>220</v>
       </c>
       <c r="C71" t="s">
-        <v>274</v>
+        <v>325</v>
       </c>
       <c r="D71" t="s">
-        <v>299</v>
+        <v>359</v>
       </c>
     </row>
     <row r="72" spans="1:4">
@@ -2282,13 +2465,13 @@
         <v>73</v>
       </c>
       <c r="B72" t="s">
-        <v>196</v>
+        <v>221</v>
       </c>
       <c r="C72" t="s">
-        <v>274</v>
+        <v>325</v>
       </c>
       <c r="D72" t="s">
-        <v>299</v>
+        <v>359</v>
       </c>
     </row>
     <row r="73" spans="1:4">
@@ -2296,13 +2479,13 @@
         <v>74</v>
       </c>
       <c r="B73" t="s">
-        <v>197</v>
+        <v>222</v>
       </c>
       <c r="C73" t="s">
-        <v>275</v>
+        <v>326</v>
       </c>
       <c r="D73" t="s">
-        <v>299</v>
+        <v>359</v>
       </c>
     </row>
     <row r="74" spans="1:4">
@@ -2310,13 +2493,13 @@
         <v>75</v>
       </c>
       <c r="B74" t="s">
-        <v>198</v>
+        <v>223</v>
       </c>
       <c r="C74" t="s">
-        <v>275</v>
+        <v>326</v>
       </c>
       <c r="D74" t="s">
-        <v>299</v>
+        <v>359</v>
       </c>
     </row>
     <row r="75" spans="1:4">
@@ -2324,13 +2507,13 @@
         <v>76</v>
       </c>
       <c r="B75" t="s">
-        <v>199</v>
+        <v>224</v>
       </c>
       <c r="C75" t="s">
-        <v>275</v>
+        <v>326</v>
       </c>
       <c r="D75" t="s">
-        <v>299</v>
+        <v>359</v>
       </c>
     </row>
     <row r="76" spans="1:4">
@@ -2338,13 +2521,13 @@
         <v>77</v>
       </c>
       <c r="B76" t="s">
-        <v>200</v>
+        <v>225</v>
       </c>
       <c r="C76" t="s">
-        <v>276</v>
+        <v>327</v>
       </c>
       <c r="D76" t="s">
-        <v>299</v>
+        <v>359</v>
       </c>
     </row>
     <row r="77" spans="1:4">
@@ -2352,13 +2535,13 @@
         <v>78</v>
       </c>
       <c r="B77" t="s">
-        <v>201</v>
+        <v>226</v>
       </c>
       <c r="C77" t="s">
-        <v>276</v>
+        <v>327</v>
       </c>
       <c r="D77" t="s">
-        <v>299</v>
+        <v>359</v>
       </c>
     </row>
     <row r="78" spans="1:4">
@@ -2366,13 +2549,13 @@
         <v>79</v>
       </c>
       <c r="B78" t="s">
-        <v>202</v>
+        <v>227</v>
       </c>
       <c r="C78" t="s">
-        <v>276</v>
+        <v>327</v>
       </c>
       <c r="D78" t="s">
-        <v>299</v>
+        <v>359</v>
       </c>
     </row>
     <row r="79" spans="1:4">
@@ -2380,13 +2563,13 @@
         <v>78</v>
       </c>
       <c r="B79" t="s">
-        <v>201</v>
+        <v>226</v>
       </c>
       <c r="C79" t="s">
-        <v>277</v>
+        <v>328</v>
       </c>
       <c r="D79" t="s">
-        <v>299</v>
+        <v>359</v>
       </c>
     </row>
     <row r="80" spans="1:4">
@@ -2394,13 +2577,13 @@
         <v>80</v>
       </c>
       <c r="B80" t="s">
-        <v>203</v>
+        <v>228</v>
       </c>
       <c r="C80" t="s">
-        <v>277</v>
+        <v>328</v>
       </c>
       <c r="D80" t="s">
-        <v>299</v>
+        <v>359</v>
       </c>
     </row>
     <row r="81" spans="1:4">
@@ -2408,13 +2591,13 @@
         <v>81</v>
       </c>
       <c r="B81" t="s">
-        <v>204</v>
+        <v>229</v>
       </c>
       <c r="C81" t="s">
-        <v>277</v>
+        <v>328</v>
       </c>
       <c r="D81" t="s">
-        <v>299</v>
+        <v>359</v>
       </c>
     </row>
     <row r="82" spans="1:4">
@@ -2422,13 +2605,13 @@
         <v>10</v>
       </c>
       <c r="B82" t="s">
-        <v>133</v>
+        <v>158</v>
       </c>
       <c r="C82" t="s">
-        <v>278</v>
+        <v>329</v>
       </c>
       <c r="D82" t="s">
-        <v>299</v>
+        <v>359</v>
       </c>
     </row>
     <row r="83" spans="1:4">
@@ -2436,13 +2619,13 @@
         <v>82</v>
       </c>
       <c r="B83" t="s">
-        <v>205</v>
+        <v>230</v>
       </c>
       <c r="C83" t="s">
-        <v>278</v>
+        <v>329</v>
       </c>
       <c r="D83" t="s">
-        <v>299</v>
+        <v>359</v>
       </c>
     </row>
     <row r="84" spans="1:4">
@@ -2450,13 +2633,13 @@
         <v>83</v>
       </c>
       <c r="B84" t="s">
-        <v>206</v>
+        <v>231</v>
       </c>
       <c r="C84" t="s">
-        <v>278</v>
+        <v>329</v>
       </c>
       <c r="D84" t="s">
-        <v>299</v>
+        <v>359</v>
       </c>
     </row>
     <row r="85" spans="1:4">
@@ -2464,13 +2647,13 @@
         <v>10</v>
       </c>
       <c r="B85" t="s">
-        <v>133</v>
+        <v>158</v>
       </c>
       <c r="C85" t="s">
-        <v>279</v>
+        <v>330</v>
       </c>
       <c r="D85" t="s">
-        <v>299</v>
+        <v>359</v>
       </c>
     </row>
     <row r="86" spans="1:4">
@@ -2478,13 +2661,13 @@
         <v>84</v>
       </c>
       <c r="B86" t="s">
-        <v>207</v>
+        <v>232</v>
       </c>
       <c r="C86" t="s">
-        <v>279</v>
+        <v>330</v>
       </c>
       <c r="D86" t="s">
-        <v>299</v>
+        <v>359</v>
       </c>
     </row>
     <row r="87" spans="1:4">
@@ -2492,13 +2675,13 @@
         <v>85</v>
       </c>
       <c r="B87" t="s">
-        <v>208</v>
+        <v>233</v>
       </c>
       <c r="C87" t="s">
-        <v>279</v>
+        <v>330</v>
       </c>
       <c r="D87" t="s">
-        <v>299</v>
+        <v>359</v>
       </c>
     </row>
     <row r="88" spans="1:4">
@@ -2506,13 +2689,13 @@
         <v>11</v>
       </c>
       <c r="B88" t="s">
-        <v>134</v>
+        <v>159</v>
       </c>
       <c r="C88" t="s">
-        <v>280</v>
+        <v>331</v>
       </c>
       <c r="D88" t="s">
-        <v>299</v>
+        <v>359</v>
       </c>
     </row>
     <row r="89" spans="1:4">
@@ -2520,13 +2703,13 @@
         <v>86</v>
       </c>
       <c r="B89" t="s">
-        <v>209</v>
+        <v>234</v>
       </c>
       <c r="C89" t="s">
-        <v>280</v>
+        <v>331</v>
       </c>
       <c r="D89" t="s">
-        <v>299</v>
+        <v>359</v>
       </c>
     </row>
     <row r="90" spans="1:4">
@@ -2534,13 +2717,13 @@
         <v>87</v>
       </c>
       <c r="B90" t="s">
-        <v>210</v>
+        <v>235</v>
       </c>
       <c r="C90" t="s">
-        <v>280</v>
+        <v>331</v>
       </c>
       <c r="D90" t="s">
-        <v>299</v>
+        <v>359</v>
       </c>
     </row>
     <row r="91" spans="1:4">
@@ -2548,13 +2731,13 @@
         <v>88</v>
       </c>
       <c r="B91" t="s">
-        <v>211</v>
+        <v>236</v>
       </c>
       <c r="C91" t="s">
-        <v>281</v>
+        <v>332</v>
       </c>
       <c r="D91" t="s">
-        <v>300</v>
+        <v>360</v>
       </c>
     </row>
     <row r="92" spans="1:4">
@@ -2562,13 +2745,13 @@
         <v>89</v>
       </c>
       <c r="B92" t="s">
-        <v>212</v>
+        <v>237</v>
       </c>
       <c r="C92" t="s">
-        <v>281</v>
+        <v>332</v>
       </c>
       <c r="D92" t="s">
-        <v>300</v>
+        <v>360</v>
       </c>
     </row>
     <row r="93" spans="1:4">
@@ -2576,13 +2759,13 @@
         <v>90</v>
       </c>
       <c r="B93" t="s">
-        <v>213</v>
+        <v>238</v>
       </c>
       <c r="C93" t="s">
-        <v>281</v>
+        <v>332</v>
       </c>
       <c r="D93" t="s">
-        <v>300</v>
+        <v>360</v>
       </c>
     </row>
     <row r="94" spans="1:4">
@@ -2590,13 +2773,13 @@
         <v>91</v>
       </c>
       <c r="B94" t="s">
-        <v>214</v>
+        <v>239</v>
       </c>
       <c r="C94" t="s">
-        <v>282</v>
+        <v>333</v>
       </c>
       <c r="D94" t="s">
-        <v>300</v>
+        <v>360</v>
       </c>
     </row>
     <row r="95" spans="1:4">
@@ -2604,13 +2787,13 @@
         <v>92</v>
       </c>
       <c r="B95" t="s">
-        <v>215</v>
+        <v>240</v>
       </c>
       <c r="C95" t="s">
-        <v>282</v>
+        <v>333</v>
       </c>
       <c r="D95" t="s">
-        <v>300</v>
+        <v>360</v>
       </c>
     </row>
     <row r="96" spans="1:4">
@@ -2618,13 +2801,13 @@
         <v>93</v>
       </c>
       <c r="B96" t="s">
-        <v>216</v>
+        <v>241</v>
       </c>
       <c r="C96" t="s">
-        <v>282</v>
+        <v>333</v>
       </c>
       <c r="D96" t="s">
-        <v>300</v>
+        <v>360</v>
       </c>
     </row>
     <row r="97" spans="1:4">
@@ -2632,13 +2815,13 @@
         <v>12</v>
       </c>
       <c r="B97" t="s">
-        <v>135</v>
+        <v>160</v>
       </c>
       <c r="C97" t="s">
-        <v>283</v>
+        <v>334</v>
       </c>
       <c r="D97" t="s">
-        <v>300</v>
+        <v>360</v>
       </c>
     </row>
     <row r="98" spans="1:4">
@@ -2646,13 +2829,13 @@
         <v>94</v>
       </c>
       <c r="B98" t="s">
-        <v>217</v>
+        <v>242</v>
       </c>
       <c r="C98" t="s">
-        <v>284</v>
+        <v>335</v>
       </c>
       <c r="D98" t="s">
-        <v>300</v>
+        <v>360</v>
       </c>
     </row>
     <row r="99" spans="1:4">
@@ -2660,13 +2843,13 @@
         <v>95</v>
       </c>
       <c r="B99" t="s">
-        <v>218</v>
+        <v>243</v>
       </c>
       <c r="C99" t="s">
-        <v>284</v>
+        <v>335</v>
       </c>
       <c r="D99" t="s">
-        <v>300</v>
+        <v>360</v>
       </c>
     </row>
     <row r="100" spans="1:4">
@@ -2674,13 +2857,13 @@
         <v>96</v>
       </c>
       <c r="B100" t="s">
-        <v>219</v>
+        <v>244</v>
       </c>
       <c r="C100" t="s">
-        <v>284</v>
+        <v>335</v>
       </c>
       <c r="D100" t="s">
-        <v>300</v>
+        <v>360</v>
       </c>
     </row>
     <row r="101" spans="1:4">
@@ -2688,13 +2871,13 @@
         <v>97</v>
       </c>
       <c r="B101" t="s">
-        <v>220</v>
+        <v>245</v>
       </c>
       <c r="C101" t="s">
-        <v>285</v>
+        <v>336</v>
       </c>
       <c r="D101" t="s">
-        <v>300</v>
+        <v>360</v>
       </c>
     </row>
     <row r="102" spans="1:4">
@@ -2702,13 +2885,13 @@
         <v>98</v>
       </c>
       <c r="B102" t="s">
-        <v>221</v>
+        <v>246</v>
       </c>
       <c r="C102" t="s">
-        <v>285</v>
+        <v>336</v>
       </c>
       <c r="D102" t="s">
-        <v>300</v>
+        <v>360</v>
       </c>
     </row>
     <row r="103" spans="1:4">
@@ -2716,13 +2899,13 @@
         <v>99</v>
       </c>
       <c r="B103" t="s">
-        <v>222</v>
+        <v>247</v>
       </c>
       <c r="C103" t="s">
-        <v>285</v>
+        <v>336</v>
       </c>
       <c r="D103" t="s">
-        <v>300</v>
+        <v>360</v>
       </c>
     </row>
     <row r="104" spans="1:4">
@@ -2730,13 +2913,13 @@
         <v>100</v>
       </c>
       <c r="B104" t="s">
-        <v>223</v>
+        <v>248</v>
       </c>
       <c r="C104" t="s">
-        <v>286</v>
+        <v>337</v>
       </c>
       <c r="D104" t="s">
-        <v>300</v>
+        <v>360</v>
       </c>
     </row>
     <row r="105" spans="1:4">
@@ -2744,13 +2927,13 @@
         <v>101</v>
       </c>
       <c r="B105" t="s">
-        <v>224</v>
+        <v>249</v>
       </c>
       <c r="C105" t="s">
-        <v>286</v>
+        <v>337</v>
       </c>
       <c r="D105" t="s">
-        <v>300</v>
+        <v>360</v>
       </c>
     </row>
     <row r="106" spans="1:4">
@@ -2758,13 +2941,13 @@
         <v>102</v>
       </c>
       <c r="B106" t="s">
-        <v>225</v>
+        <v>250</v>
       </c>
       <c r="C106" t="s">
-        <v>286</v>
+        <v>337</v>
       </c>
       <c r="D106" t="s">
-        <v>300</v>
+        <v>360</v>
       </c>
     </row>
     <row r="107" spans="1:4">
@@ -2772,13 +2955,13 @@
         <v>103</v>
       </c>
       <c r="B107" t="s">
-        <v>226</v>
+        <v>251</v>
       </c>
       <c r="C107" t="s">
-        <v>287</v>
+        <v>338</v>
       </c>
       <c r="D107" t="s">
-        <v>300</v>
+        <v>360</v>
       </c>
     </row>
     <row r="108" spans="1:4">
@@ -2786,13 +2969,13 @@
         <v>104</v>
       </c>
       <c r="B108" t="s">
-        <v>227</v>
+        <v>252</v>
       </c>
       <c r="C108" t="s">
-        <v>287</v>
+        <v>338</v>
       </c>
       <c r="D108" t="s">
-        <v>300</v>
+        <v>360</v>
       </c>
     </row>
     <row r="109" spans="1:4">
@@ -2800,13 +2983,13 @@
         <v>105</v>
       </c>
       <c r="B109" t="s">
-        <v>228</v>
+        <v>253</v>
       </c>
       <c r="C109" t="s">
-        <v>287</v>
+        <v>338</v>
       </c>
       <c r="D109" t="s">
-        <v>300</v>
+        <v>360</v>
       </c>
     </row>
     <row r="110" spans="1:4">
@@ -2814,13 +2997,13 @@
         <v>16</v>
       </c>
       <c r="B110" t="s">
-        <v>139</v>
+        <v>164</v>
       </c>
       <c r="C110" t="s">
-        <v>288</v>
+        <v>339</v>
       </c>
       <c r="D110" t="s">
-        <v>300</v>
+        <v>360</v>
       </c>
     </row>
     <row r="111" spans="1:4">
@@ -2828,13 +3011,13 @@
         <v>106</v>
       </c>
       <c r="B111" t="s">
-        <v>229</v>
+        <v>254</v>
       </c>
       <c r="C111" t="s">
-        <v>288</v>
+        <v>339</v>
       </c>
       <c r="D111" t="s">
-        <v>300</v>
+        <v>360</v>
       </c>
     </row>
     <row r="112" spans="1:4">
@@ -2842,13 +3025,13 @@
         <v>107</v>
       </c>
       <c r="B112" t="s">
-        <v>230</v>
+        <v>255</v>
       </c>
       <c r="C112" t="s">
-        <v>288</v>
+        <v>339</v>
       </c>
       <c r="D112" t="s">
-        <v>300</v>
+        <v>360</v>
       </c>
     </row>
     <row r="113" spans="1:4">
@@ -2856,13 +3039,13 @@
         <v>16</v>
       </c>
       <c r="B113" t="s">
-        <v>139</v>
+        <v>164</v>
       </c>
       <c r="C113" t="s">
-        <v>289</v>
+        <v>340</v>
       </c>
       <c r="D113" t="s">
-        <v>300</v>
+        <v>360</v>
       </c>
     </row>
     <row r="114" spans="1:4">
@@ -2870,13 +3053,13 @@
         <v>108</v>
       </c>
       <c r="B114" t="s">
-        <v>231</v>
+        <v>256</v>
       </c>
       <c r="C114" t="s">
-        <v>289</v>
+        <v>340</v>
       </c>
       <c r="D114" t="s">
-        <v>300</v>
+        <v>360</v>
       </c>
     </row>
     <row r="115" spans="1:4">
@@ -2884,13 +3067,13 @@
         <v>109</v>
       </c>
       <c r="B115" t="s">
-        <v>232</v>
+        <v>257</v>
       </c>
       <c r="C115" t="s">
-        <v>289</v>
+        <v>340</v>
       </c>
       <c r="D115" t="s">
-        <v>300</v>
+        <v>360</v>
       </c>
     </row>
     <row r="116" spans="1:4">
@@ -2898,13 +3081,13 @@
         <v>18</v>
       </c>
       <c r="B116" t="s">
-        <v>141</v>
+        <v>166</v>
       </c>
       <c r="C116" t="s">
-        <v>290</v>
+        <v>341</v>
       </c>
       <c r="D116" t="s">
-        <v>300</v>
+        <v>360</v>
       </c>
     </row>
     <row r="117" spans="1:4">
@@ -2912,13 +3095,13 @@
         <v>110</v>
       </c>
       <c r="B117" t="s">
-        <v>233</v>
+        <v>258</v>
       </c>
       <c r="C117" t="s">
-        <v>290</v>
+        <v>341</v>
       </c>
       <c r="D117" t="s">
-        <v>300</v>
+        <v>360</v>
       </c>
     </row>
     <row r="118" spans="1:4">
@@ -2926,13 +3109,13 @@
         <v>111</v>
       </c>
       <c r="B118" t="s">
-        <v>234</v>
+        <v>259</v>
       </c>
       <c r="C118" t="s">
-        <v>290</v>
+        <v>341</v>
       </c>
       <c r="D118" t="s">
-        <v>300</v>
+        <v>360</v>
       </c>
     </row>
     <row r="119" spans="1:4">
@@ -2940,13 +3123,13 @@
         <v>18</v>
       </c>
       <c r="B119" t="s">
-        <v>141</v>
+        <v>166</v>
       </c>
       <c r="C119" t="s">
-        <v>291</v>
+        <v>342</v>
       </c>
       <c r="D119" t="s">
-        <v>300</v>
+        <v>360</v>
       </c>
     </row>
     <row r="120" spans="1:4">
@@ -2954,13 +3137,13 @@
         <v>112</v>
       </c>
       <c r="B120" t="s">
-        <v>235</v>
+        <v>260</v>
       </c>
       <c r="C120" t="s">
-        <v>291</v>
+        <v>342</v>
       </c>
       <c r="D120" t="s">
-        <v>300</v>
+        <v>360</v>
       </c>
     </row>
     <row r="121" spans="1:4">
@@ -2968,13 +3151,13 @@
         <v>113</v>
       </c>
       <c r="B121" t="s">
-        <v>236</v>
+        <v>261</v>
       </c>
       <c r="C121" t="s">
-        <v>291</v>
+        <v>342</v>
       </c>
       <c r="D121" t="s">
-        <v>300</v>
+        <v>360</v>
       </c>
     </row>
     <row r="122" spans="1:4">
@@ -2982,13 +3165,13 @@
         <v>114</v>
       </c>
       <c r="B122" t="s">
-        <v>237</v>
+        <v>262</v>
       </c>
       <c r="C122" t="s">
-        <v>292</v>
+        <v>343</v>
       </c>
       <c r="D122" t="s">
-        <v>301</v>
+        <v>361</v>
       </c>
     </row>
     <row r="123" spans="1:4">
@@ -2996,13 +3179,13 @@
         <v>19</v>
       </c>
       <c r="B123" t="s">
-        <v>142</v>
+        <v>167</v>
       </c>
       <c r="C123" t="s">
-        <v>292</v>
+        <v>343</v>
       </c>
       <c r="D123" t="s">
-        <v>301</v>
+        <v>361</v>
       </c>
     </row>
     <row r="124" spans="1:4">
@@ -3010,13 +3193,13 @@
         <v>115</v>
       </c>
       <c r="B124" t="s">
-        <v>238</v>
+        <v>263</v>
       </c>
       <c r="C124" t="s">
-        <v>292</v>
+        <v>343</v>
       </c>
       <c r="D124" t="s">
-        <v>301</v>
+        <v>361</v>
       </c>
     </row>
     <row r="125" spans="1:4">
@@ -3024,13 +3207,13 @@
         <v>116</v>
       </c>
       <c r="B125" t="s">
-        <v>239</v>
+        <v>264</v>
       </c>
       <c r="C125" t="s">
-        <v>293</v>
+        <v>344</v>
       </c>
       <c r="D125" t="s">
-        <v>301</v>
+        <v>361</v>
       </c>
     </row>
     <row r="126" spans="1:4">
@@ -3038,13 +3221,13 @@
         <v>117</v>
       </c>
       <c r="B126" t="s">
-        <v>240</v>
+        <v>265</v>
       </c>
       <c r="C126" t="s">
-        <v>293</v>
+        <v>344</v>
       </c>
       <c r="D126" t="s">
-        <v>301</v>
+        <v>361</v>
       </c>
     </row>
     <row r="127" spans="1:4">
@@ -3052,13 +3235,13 @@
         <v>118</v>
       </c>
       <c r="B127" t="s">
-        <v>241</v>
+        <v>266</v>
       </c>
       <c r="C127" t="s">
-        <v>293</v>
+        <v>344</v>
       </c>
       <c r="D127" t="s">
-        <v>301</v>
+        <v>361</v>
       </c>
     </row>
     <row r="128" spans="1:4">
@@ -3066,13 +3249,13 @@
         <v>20</v>
       </c>
       <c r="B128" t="s">
-        <v>143</v>
+        <v>168</v>
       </c>
       <c r="C128" t="s">
-        <v>294</v>
+        <v>345</v>
       </c>
       <c r="D128" t="s">
-        <v>301</v>
+        <v>361</v>
       </c>
     </row>
     <row r="129" spans="1:4">
@@ -3080,13 +3263,13 @@
         <v>119</v>
       </c>
       <c r="B129" t="s">
-        <v>242</v>
+        <v>267</v>
       </c>
       <c r="C129" t="s">
-        <v>294</v>
+        <v>345</v>
       </c>
       <c r="D129" t="s">
-        <v>301</v>
+        <v>361</v>
       </c>
     </row>
     <row r="130" spans="1:4">
@@ -3094,13 +3277,13 @@
         <v>120</v>
       </c>
       <c r="B130" t="s">
-        <v>243</v>
+        <v>268</v>
       </c>
       <c r="C130" t="s">
-        <v>294</v>
+        <v>345</v>
       </c>
       <c r="D130" t="s">
-        <v>301</v>
+        <v>361</v>
       </c>
     </row>
     <row r="131" spans="1:4">
@@ -3108,13 +3291,13 @@
         <v>121</v>
       </c>
       <c r="B131" t="s">
-        <v>244</v>
+        <v>269</v>
       </c>
       <c r="C131" t="s">
-        <v>295</v>
+        <v>346</v>
       </c>
       <c r="D131" t="s">
-        <v>301</v>
+        <v>361</v>
       </c>
     </row>
     <row r="132" spans="1:4">
@@ -3122,13 +3305,13 @@
         <v>122</v>
       </c>
       <c r="B132" t="s">
-        <v>245</v>
+        <v>270</v>
       </c>
       <c r="C132" t="s">
-        <v>295</v>
+        <v>346</v>
       </c>
       <c r="D132" t="s">
-        <v>301</v>
+        <v>361</v>
       </c>
     </row>
     <row r="133" spans="1:4">
@@ -3136,13 +3319,13 @@
         <v>123</v>
       </c>
       <c r="B133" t="s">
-        <v>246</v>
+        <v>271</v>
       </c>
       <c r="C133" t="s">
-        <v>295</v>
+        <v>346</v>
       </c>
       <c r="D133" t="s">
-        <v>301</v>
+        <v>361</v>
       </c>
     </row>
     <row r="134" spans="1:4">
@@ -3150,13 +3333,13 @@
         <v>124</v>
       </c>
       <c r="B134" t="s">
-        <v>247</v>
+        <v>272</v>
       </c>
       <c r="C134" t="s">
-        <v>296</v>
+        <v>347</v>
       </c>
       <c r="D134" t="s">
-        <v>301</v>
+        <v>361</v>
       </c>
     </row>
     <row r="135" spans="1:4">
@@ -3164,13 +3347,13 @@
         <v>125</v>
       </c>
       <c r="B135" t="s">
-        <v>248</v>
+        <v>273</v>
       </c>
       <c r="C135" t="s">
-        <v>296</v>
+        <v>347</v>
       </c>
       <c r="D135" t="s">
-        <v>301</v>
+        <v>361</v>
       </c>
     </row>
     <row r="136" spans="1:4">
@@ -3178,13 +3361,374 @@
         <v>126</v>
       </c>
       <c r="B136" t="s">
-        <v>249</v>
+        <v>274</v>
       </c>
       <c r="C136" t="s">
+        <v>347</v>
+      </c>
+      <c r="D136" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="137" spans="1:4">
+      <c r="A137" t="s">
+        <v>127</v>
+      </c>
+      <c r="B137" t="s">
+        <v>275</v>
+      </c>
+      <c r="C137" t="s">
+        <v>348</v>
+      </c>
+      <c r="D137" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="138" spans="1:4">
+      <c r="A138" t="s">
+        <v>128</v>
+      </c>
+      <c r="B138" t="s">
+        <v>276</v>
+      </c>
+      <c r="C138" t="s">
+        <v>348</v>
+      </c>
+      <c r="D138" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="139" spans="1:4">
+      <c r="A139" t="s">
+        <v>129</v>
+      </c>
+      <c r="B139" t="s">
+        <v>277</v>
+      </c>
+      <c r="C139" t="s">
+        <v>348</v>
+      </c>
+      <c r="D139" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="140" spans="1:4">
+      <c r="A140" t="s">
+        <v>130</v>
+      </c>
+      <c r="B140" t="s">
+        <v>278</v>
+      </c>
+      <c r="C140" t="s">
+        <v>349</v>
+      </c>
+      <c r="D140" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="141" spans="1:4">
+      <c r="A141" t="s">
+        <v>131</v>
+      </c>
+      <c r="B141" t="s">
+        <v>279</v>
+      </c>
+      <c r="C141" t="s">
+        <v>349</v>
+      </c>
+      <c r="D141" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="142" spans="1:4">
+      <c r="A142" t="s">
+        <v>132</v>
+      </c>
+      <c r="B142" t="s">
+        <v>280</v>
+      </c>
+      <c r="C142" t="s">
+        <v>349</v>
+      </c>
+      <c r="D142" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="143" spans="1:4">
+      <c r="A143" t="s">
+        <v>133</v>
+      </c>
+      <c r="B143" t="s">
+        <v>281</v>
+      </c>
+      <c r="C143" t="s">
+        <v>350</v>
+      </c>
+      <c r="D143" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="144" spans="1:4">
+      <c r="A144" t="s">
+        <v>134</v>
+      </c>
+      <c r="B144" t="s">
+        <v>282</v>
+      </c>
+      <c r="C144" t="s">
+        <v>350</v>
+      </c>
+      <c r="D144" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="145" spans="1:4">
+      <c r="A145" t="s">
+        <v>135</v>
+      </c>
+      <c r="B145" t="s">
+        <v>283</v>
+      </c>
+      <c r="C145" t="s">
+        <v>350</v>
+      </c>
+      <c r="D145" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="146" spans="1:4">
+      <c r="A146" t="s">
+        <v>136</v>
+      </c>
+      <c r="B146" t="s">
+        <v>284</v>
+      </c>
+      <c r="C146" t="s">
+        <v>351</v>
+      </c>
+      <c r="D146" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="147" spans="1:4">
+      <c r="A147" t="s">
+        <v>137</v>
+      </c>
+      <c r="B147" t="s">
+        <v>285</v>
+      </c>
+      <c r="C147" t="s">
+        <v>351</v>
+      </c>
+      <c r="D147" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="148" spans="1:4">
+      <c r="A148" t="s">
+        <v>138</v>
+      </c>
+      <c r="B148" t="s">
+        <v>286</v>
+      </c>
+      <c r="C148" t="s">
+        <v>351</v>
+      </c>
+      <c r="D148" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="149" spans="1:4">
+      <c r="A149" t="s">
+        <v>139</v>
+      </c>
+      <c r="B149" t="s">
+        <v>287</v>
+      </c>
+      <c r="C149" t="s">
+        <v>352</v>
+      </c>
+      <c r="D149" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="150" spans="1:4">
+      <c r="A150" t="s">
+        <v>140</v>
+      </c>
+      <c r="B150" t="s">
+        <v>288</v>
+      </c>
+      <c r="C150" t="s">
+        <v>352</v>
+      </c>
+      <c r="D150" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="151" spans="1:4">
+      <c r="A151" t="s">
+        <v>141</v>
+      </c>
+      <c r="B151" t="s">
+        <v>289</v>
+      </c>
+      <c r="C151" t="s">
+        <v>352</v>
+      </c>
+      <c r="D151" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="152" spans="1:4">
+      <c r="A152" t="s">
+        <v>142</v>
+      </c>
+      <c r="B152" t="s">
+        <v>290</v>
+      </c>
+      <c r="C152" t="s">
+        <v>353</v>
+      </c>
+      <c r="D152" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="153" spans="1:4">
+      <c r="A153" t="s">
+        <v>143</v>
+      </c>
+      <c r="B153" t="s">
+        <v>291</v>
+      </c>
+      <c r="C153" t="s">
+        <v>353</v>
+      </c>
+      <c r="D153" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="154" spans="1:4">
+      <c r="A154" t="s">
+        <v>144</v>
+      </c>
+      <c r="B154" t="s">
+        <v>292</v>
+      </c>
+      <c r="C154" t="s">
+        <v>353</v>
+      </c>
+      <c r="D154" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="155" spans="1:4">
+      <c r="A155" t="s">
+        <v>145</v>
+      </c>
+      <c r="B155" t="s">
+        <v>293</v>
+      </c>
+      <c r="C155" t="s">
+        <v>354</v>
+      </c>
+      <c r="D155" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="156" spans="1:4">
+      <c r="A156" t="s">
+        <v>146</v>
+      </c>
+      <c r="B156" t="s">
+        <v>294</v>
+      </c>
+      <c r="C156" t="s">
+        <v>354</v>
+      </c>
+      <c r="D156" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="157" spans="1:4">
+      <c r="A157" t="s">
+        <v>147</v>
+      </c>
+      <c r="B157" t="s">
+        <v>295</v>
+      </c>
+      <c r="C157" t="s">
+        <v>354</v>
+      </c>
+      <c r="D157" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="158" spans="1:4">
+      <c r="A158" t="s">
+        <v>148</v>
+      </c>
+      <c r="B158" t="s">
         <v>296</v>
       </c>
-      <c r="D136" t="s">
-        <v>301</v>
+      <c r="C158" t="s">
+        <v>355</v>
+      </c>
+      <c r="D158" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="159" spans="1:4">
+      <c r="A159" t="s">
+        <v>149</v>
+      </c>
+      <c r="B159" t="s">
+        <v>297</v>
+      </c>
+      <c r="C159" t="s">
+        <v>355</v>
+      </c>
+      <c r="D159" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="160" spans="1:4">
+      <c r="A160" t="s">
+        <v>150</v>
+      </c>
+      <c r="B160" t="s">
+        <v>298</v>
+      </c>
+      <c r="C160" t="s">
+        <v>355</v>
+      </c>
+      <c r="D160" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="161" spans="1:4">
+      <c r="A161" t="s">
+        <v>151</v>
+      </c>
+      <c r="B161" t="s">
+        <v>299</v>
+      </c>
+      <c r="C161" t="s">
+        <v>356</v>
+      </c>
+      <c r="D161" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="162" spans="1:4">
+      <c r="B162" t="s">
+        <v>300</v>
+      </c>
+      <c r="C162" t="s">
+        <v>356</v>
+      </c>
+      <c r="D162" t="s">
+        <v>362</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changed writing to 14 days prior and updated DBs
</commit_message>
<xml_diff>
--- a/Databases/中文_sentences.xlsx
+++ b/Databases/中文_sentences.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="647" uniqueCount="363">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="847" uniqueCount="481">
   <si>
     <t>FOREIGN</t>
   </si>
@@ -472,6 +472,156 @@
     <t xml:space="preserve">习惯是后天养成的。  </t>
   </si>
   <si>
+    <t xml:space="preserve">你看，我有好消息。  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">最近没什么好消息。  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">报纸的头版有好消息。  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">人们热烈鼓掌，掌声经久不衰。  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">全校师生热烈欢迎新校长。  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">会上展开了热烈的讨论。  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">舆论界对世界两大汽车制造商的合作褒贬不一。  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">人们对他褒贬不一。  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">这次试飞的反映褒贬不一。  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">仿效我们的做法，你就可以一举两得。  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">我昨天想出去走走，顺便带上了我的狗，真是一举两得啊。  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">一举两得。  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">他需要鼓励。  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">家长应该鼓励孩子。  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">他们流露出一丝鼓励。  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">不战则已，战则必胜。  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">公则生明，廉则生威。 - 朱舜水  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">我没依照任何参考。  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">他参考了另一个文献。  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">以上观点仅供参考。  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">她侵犯了我的隐私。  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">这侵犯了我的个人权利。  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">他们签定了互不侵犯条约。  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">丹尼斯涉嫌谋杀。  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">他因涉嫌贪污被逮捕。  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">他因涉嫌是美国间谍而被逮捕。  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">不要歧视残疾人。  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">我们将会反对歧视。  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">主要党派都精通于种族歧视。  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">像成功人士一样思考。  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">这是病残人士的专座。  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">这张纸业余人士也能贴上去。  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">亦或是漠不关心。  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">亦或能够使之蒸发。  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">或者倾听，亦或交流。  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">一阵令人焦虑的沉默。  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">他们焦虑不安，不断跳跃。  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">她感到焦虑，哪都不对劲。  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">我没有恶意。  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">他对她没有恶意。  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">他受到了恶意攻击。  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">我对市场营销相当了解。  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">这家公司高度重视市场营销。  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">营销和广告公司应当扬长避短。  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">这书值得买。  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">很值得做…  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">值得注意的是…  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">儒家思想提倡忠恕。  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">国家提倡按时缴纳中央税。  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">教育机构提倡安全使用互联网。  </t>
+  </si>
+  <si>
     <t>I didn't even mind the lack of an in-flight meal service.</t>
   </si>
   <si>
@@ -919,6 +1069,156 @@
     <t>Yǎngchéng jiàoyù hěn zhòngyào，yào zhùyì péiyǎng háizi de liánghǎo xíguàn.</t>
   </si>
   <si>
+    <t>Guess what，I've got good news.</t>
+  </si>
+  <si>
+    <t>Good news has been thin on the ground lately.</t>
+  </si>
+  <si>
+    <t>The newspaper had good news on its front page.</t>
+  </si>
+  <si>
+    <t>The crowd applauded to the echo.</t>
+  </si>
+  <si>
+    <t>The whole university welcomed the new principal warmly.</t>
+  </si>
+  <si>
+    <t>Heated discussions occurred in the conference.</t>
+  </si>
+  <si>
+    <t>The press has different attitudes towards cooperation between the world's two major automobile manufacturers.</t>
+  </si>
+  <si>
+    <t>People pass different judgements on him.</t>
+  </si>
+  <si>
+    <t>Reaction to the test flight was mixed.</t>
+  </si>
+  <si>
+    <t>You could kill two birds with one stone by following our example.</t>
+  </si>
+  <si>
+    <t>I wanted to go for a walk yesterday and by taking my dog with me, I killed two birds with one stone.</t>
+  </si>
+  <si>
+    <t>You can kill two birds with one stone.</t>
+  </si>
+  <si>
+    <t>He needs encouragement.'</t>
+  </si>
+  <si>
+    <t>Parents should encourage their children.</t>
+  </si>
+  <si>
+    <t>They hold out little encouragement.</t>
+  </si>
+  <si>
+    <t>If you don't fight, then fine. If you do fight, fight to win.</t>
+  </si>
+  <si>
+    <t>Honesty produces justice, while probity brings about power.</t>
+  </si>
+  <si>
+    <t>I don't go by anything at all.</t>
+  </si>
+  <si>
+    <t>He appealed to another document.</t>
+  </si>
+  <si>
+    <t>The above advice is only for reference.</t>
+  </si>
+  <si>
+    <t>She is trespassing upon my privacy.</t>
+  </si>
+  <si>
+    <t>This impinges on my rights as an individual.</t>
+  </si>
+  <si>
+    <t>They signed a nonaggression pact.</t>
+  </si>
+  <si>
+    <t>Dennis is suspected of murder.</t>
+  </si>
+  <si>
+    <t>He was arrested on suspicion of corruption.</t>
+  </si>
+  <si>
+    <t>He was arrested on suspicion of being an American spy.</t>
+  </si>
+  <si>
+    <t>Don't discriminate against handicapped people.</t>
+  </si>
+  <si>
+    <t>We've got it within us to react against prejudice.</t>
+  </si>
+  <si>
+    <t>The main parties are steeped in racial divisions.</t>
+  </si>
+  <si>
+    <t>Think like a winner.</t>
+  </si>
+  <si>
+    <t>This seat is specially reserved for handicapped people.</t>
+  </si>
+  <si>
+    <t>The paper could be pasted up by amateurs.</t>
+  </si>
+  <si>
+    <t>Or simply indifferent.</t>
+  </si>
+  <si>
+    <t>Or vaporize it, would be  like it.</t>
+  </si>
+  <si>
+    <t>Or listen. Or try to have an exchange.</t>
+  </si>
+  <si>
+    <t>There was a suspenseful silence.</t>
+  </si>
+  <si>
+    <t>They flutter about nervously in staccato hops.</t>
+  </si>
+  <si>
+    <t>She felt restless, at odds with herself.</t>
+  </si>
+  <si>
+    <t>There were no hard feelings on my part.</t>
+  </si>
+  <si>
+    <t>He wished her no ill.</t>
+  </si>
+  <si>
+    <t>He was viciously attacked.</t>
+  </si>
+  <si>
+    <t>I have substantial understanding of marketing.</t>
+  </si>
+  <si>
+    <t>This company puts a high value on marketing.</t>
+  </si>
+  <si>
+    <t>Marketers and advertisers who want to be successful on the Net should be playing to its strength, not its weakness.</t>
+  </si>
+  <si>
+    <t>This book is worth buying.</t>
+  </si>
+  <si>
+    <t>it would be (well) worth doing...</t>
+  </si>
+  <si>
+    <t>it is notable that...</t>
+  </si>
+  <si>
+    <t>Confucianists advocate the idea of loyalty and consideration.</t>
+  </si>
+  <si>
+    <t>The State encourages paying the central tax on time.</t>
+  </si>
+  <si>
+    <t>Education providers advocate safe use of the internet.</t>
+  </si>
+  <si>
     <t>餐饮</t>
   </si>
   <si>
@@ -1087,6 +1387,57 @@
     <t>养成</t>
   </si>
   <si>
+    <t>消息</t>
+  </si>
+  <si>
+    <t>热烈</t>
+  </si>
+  <si>
+    <t>褒贬不一</t>
+  </si>
+  <si>
+    <t>一举两得</t>
+  </si>
+  <si>
+    <t>鼓励</t>
+  </si>
+  <si>
+    <t>则</t>
+  </si>
+  <si>
+    <t>参考</t>
+  </si>
+  <si>
+    <t>侵犯</t>
+  </si>
+  <si>
+    <t>涉嫌</t>
+  </si>
+  <si>
+    <t>歧视</t>
+  </si>
+  <si>
+    <t>人士</t>
+  </si>
+  <si>
+    <t>亦或</t>
+  </si>
+  <si>
+    <t>焦虑</t>
+  </si>
+  <si>
+    <t>恶意</t>
+  </si>
+  <si>
+    <t>营销</t>
+  </si>
+  <si>
+    <t>值得</t>
+  </si>
+  <si>
+    <t>提倡</t>
+  </si>
+  <si>
     <t>2020-11-25</t>
   </si>
   <si>
@@ -1103,6 +1454,9 @@
   </si>
   <si>
     <t>2020-12-02</t>
+  </si>
+  <si>
+    <t>2020-12-03</t>
   </si>
 </sst>
 </file>
@@ -1460,7 +1814,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D162"/>
+  <dimension ref="A1:D212"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1485,13 +1839,13 @@
         <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>152</v>
+        <v>202</v>
       </c>
       <c r="C2" t="s">
-        <v>301</v>
+        <v>401</v>
       </c>
       <c r="D2" t="s">
-        <v>357</v>
+        <v>474</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -1499,13 +1853,13 @@
         <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>153</v>
+        <v>203</v>
       </c>
       <c r="C3" t="s">
-        <v>301</v>
+        <v>401</v>
       </c>
       <c r="D3" t="s">
-        <v>357</v>
+        <v>474</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -1513,13 +1867,13 @@
         <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>154</v>
+        <v>204</v>
       </c>
       <c r="C4" t="s">
-        <v>301</v>
+        <v>401</v>
       </c>
       <c r="D4" t="s">
-        <v>357</v>
+        <v>474</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -1527,13 +1881,13 @@
         <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>155</v>
+        <v>205</v>
       </c>
       <c r="C5" t="s">
-        <v>302</v>
+        <v>402</v>
       </c>
       <c r="D5" t="s">
-        <v>357</v>
+        <v>474</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -1541,13 +1895,13 @@
         <v>8</v>
       </c>
       <c r="B6" t="s">
-        <v>156</v>
+        <v>206</v>
       </c>
       <c r="C6" t="s">
-        <v>302</v>
+        <v>402</v>
       </c>
       <c r="D6" t="s">
-        <v>357</v>
+        <v>474</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -1555,13 +1909,13 @@
         <v>9</v>
       </c>
       <c r="B7" t="s">
-        <v>157</v>
+        <v>207</v>
       </c>
       <c r="C7" t="s">
-        <v>302</v>
+        <v>402</v>
       </c>
       <c r="D7" t="s">
-        <v>357</v>
+        <v>474</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -1569,13 +1923,13 @@
         <v>10</v>
       </c>
       <c r="B8" t="s">
-        <v>158</v>
+        <v>208</v>
       </c>
       <c r="C8" t="s">
-        <v>303</v>
+        <v>403</v>
       </c>
       <c r="D8" t="s">
-        <v>357</v>
+        <v>474</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -1583,13 +1937,13 @@
         <v>11</v>
       </c>
       <c r="B9" t="s">
-        <v>159</v>
+        <v>209</v>
       </c>
       <c r="C9" t="s">
-        <v>303</v>
+        <v>403</v>
       </c>
       <c r="D9" t="s">
-        <v>357</v>
+        <v>474</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -1597,13 +1951,13 @@
         <v>12</v>
       </c>
       <c r="B10" t="s">
-        <v>160</v>
+        <v>210</v>
       </c>
       <c r="C10" t="s">
-        <v>303</v>
+        <v>403</v>
       </c>
       <c r="D10" t="s">
-        <v>357</v>
+        <v>474</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -1611,13 +1965,13 @@
         <v>13</v>
       </c>
       <c r="B11" t="s">
-        <v>161</v>
+        <v>211</v>
       </c>
       <c r="C11" t="s">
-        <v>304</v>
+        <v>404</v>
       </c>
       <c r="D11" t="s">
-        <v>357</v>
+        <v>474</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -1625,13 +1979,13 @@
         <v>14</v>
       </c>
       <c r="B12" t="s">
-        <v>162</v>
+        <v>212</v>
       </c>
       <c r="C12" t="s">
-        <v>304</v>
+        <v>404</v>
       </c>
       <c r="D12" t="s">
-        <v>357</v>
+        <v>474</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -1639,13 +1993,13 @@
         <v>15</v>
       </c>
       <c r="B13" t="s">
-        <v>163</v>
+        <v>213</v>
       </c>
       <c r="C13" t="s">
-        <v>304</v>
+        <v>404</v>
       </c>
       <c r="D13" t="s">
-        <v>357</v>
+        <v>474</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -1653,13 +2007,13 @@
         <v>16</v>
       </c>
       <c r="B14" t="s">
-        <v>164</v>
+        <v>214</v>
       </c>
       <c r="C14" t="s">
-        <v>305</v>
+        <v>405</v>
       </c>
       <c r="D14" t="s">
-        <v>357</v>
+        <v>474</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -1667,13 +2021,13 @@
         <v>17</v>
       </c>
       <c r="B15" t="s">
-        <v>165</v>
+        <v>215</v>
       </c>
       <c r="C15" t="s">
-        <v>305</v>
+        <v>405</v>
       </c>
       <c r="D15" t="s">
-        <v>357</v>
+        <v>474</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -1681,13 +2035,13 @@
         <v>18</v>
       </c>
       <c r="B16" t="s">
-        <v>166</v>
+        <v>216</v>
       </c>
       <c r="C16" t="s">
-        <v>305</v>
+        <v>405</v>
       </c>
       <c r="D16" t="s">
-        <v>357</v>
+        <v>474</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -1695,13 +2049,13 @@
         <v>19</v>
       </c>
       <c r="B17" t="s">
-        <v>167</v>
+        <v>217</v>
       </c>
       <c r="C17" t="s">
-        <v>306</v>
+        <v>406</v>
       </c>
       <c r="D17" t="s">
-        <v>357</v>
+        <v>474</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -1709,13 +2063,13 @@
         <v>20</v>
       </c>
       <c r="B18" t="s">
-        <v>168</v>
+        <v>218</v>
       </c>
       <c r="C18" t="s">
-        <v>306</v>
+        <v>406</v>
       </c>
       <c r="D18" t="s">
-        <v>357</v>
+        <v>474</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -1723,13 +2077,13 @@
         <v>21</v>
       </c>
       <c r="B19" t="s">
-        <v>169</v>
+        <v>219</v>
       </c>
       <c r="C19" t="s">
-        <v>306</v>
+        <v>406</v>
       </c>
       <c r="D19" t="s">
-        <v>357</v>
+        <v>474</v>
       </c>
     </row>
     <row r="20" spans="1:4">
@@ -1737,13 +2091,13 @@
         <v>22</v>
       </c>
       <c r="B20" t="s">
-        <v>170</v>
+        <v>220</v>
       </c>
       <c r="C20" t="s">
-        <v>307</v>
+        <v>407</v>
       </c>
       <c r="D20" t="s">
-        <v>357</v>
+        <v>474</v>
       </c>
     </row>
     <row r="21" spans="1:4">
@@ -1751,13 +2105,13 @@
         <v>23</v>
       </c>
       <c r="B21" t="s">
-        <v>171</v>
+        <v>221</v>
       </c>
       <c r="C21" t="s">
-        <v>307</v>
+        <v>407</v>
       </c>
       <c r="D21" t="s">
-        <v>357</v>
+        <v>474</v>
       </c>
     </row>
     <row r="22" spans="1:4">
@@ -1765,13 +2119,13 @@
         <v>24</v>
       </c>
       <c r="B22" t="s">
-        <v>172</v>
+        <v>222</v>
       </c>
       <c r="C22" t="s">
-        <v>307</v>
+        <v>407</v>
       </c>
       <c r="D22" t="s">
-        <v>357</v>
+        <v>474</v>
       </c>
     </row>
     <row r="23" spans="1:4">
@@ -1779,13 +2133,13 @@
         <v>25</v>
       </c>
       <c r="B23" t="s">
-        <v>173</v>
+        <v>223</v>
       </c>
       <c r="C23" t="s">
-        <v>308</v>
+        <v>408</v>
       </c>
       <c r="D23" t="s">
-        <v>357</v>
+        <v>474</v>
       </c>
     </row>
     <row r="24" spans="1:4">
@@ -1793,13 +2147,13 @@
         <v>26</v>
       </c>
       <c r="B24" t="s">
-        <v>174</v>
+        <v>224</v>
       </c>
       <c r="C24" t="s">
-        <v>308</v>
+        <v>408</v>
       </c>
       <c r="D24" t="s">
-        <v>357</v>
+        <v>474</v>
       </c>
     </row>
     <row r="25" spans="1:4">
@@ -1807,13 +2161,13 @@
         <v>27</v>
       </c>
       <c r="B25" t="s">
-        <v>175</v>
+        <v>225</v>
       </c>
       <c r="C25" t="s">
-        <v>308</v>
+        <v>408</v>
       </c>
       <c r="D25" t="s">
-        <v>357</v>
+        <v>474</v>
       </c>
     </row>
     <row r="26" spans="1:4">
@@ -1821,13 +2175,13 @@
         <v>28</v>
       </c>
       <c r="B26" t="s">
-        <v>176</v>
+        <v>226</v>
       </c>
       <c r="C26" t="s">
-        <v>309</v>
+        <v>409</v>
       </c>
       <c r="D26" t="s">
-        <v>357</v>
+        <v>474</v>
       </c>
     </row>
     <row r="27" spans="1:4">
@@ -1835,13 +2189,13 @@
         <v>29</v>
       </c>
       <c r="B27" t="s">
-        <v>177</v>
+        <v>227</v>
       </c>
       <c r="C27" t="s">
-        <v>309</v>
+        <v>409</v>
       </c>
       <c r="D27" t="s">
-        <v>357</v>
+        <v>474</v>
       </c>
     </row>
     <row r="28" spans="1:4">
@@ -1849,13 +2203,13 @@
         <v>30</v>
       </c>
       <c r="B28" t="s">
-        <v>178</v>
+        <v>228</v>
       </c>
       <c r="C28" t="s">
-        <v>309</v>
+        <v>409</v>
       </c>
       <c r="D28" t="s">
-        <v>357</v>
+        <v>474</v>
       </c>
     </row>
     <row r="29" spans="1:4">
@@ -1863,13 +2217,13 @@
         <v>31</v>
       </c>
       <c r="B29" t="s">
-        <v>179</v>
+        <v>229</v>
       </c>
       <c r="C29" t="s">
-        <v>310</v>
+        <v>410</v>
       </c>
       <c r="D29" t="s">
-        <v>358</v>
+        <v>475</v>
       </c>
     </row>
     <row r="30" spans="1:4">
@@ -1877,13 +2231,13 @@
         <v>32</v>
       </c>
       <c r="B30" t="s">
-        <v>180</v>
+        <v>230</v>
       </c>
       <c r="C30" t="s">
-        <v>310</v>
+        <v>410</v>
       </c>
       <c r="D30" t="s">
-        <v>358</v>
+        <v>475</v>
       </c>
     </row>
     <row r="31" spans="1:4">
@@ -1891,13 +2245,13 @@
         <v>33</v>
       </c>
       <c r="B31" t="s">
-        <v>181</v>
+        <v>231</v>
       </c>
       <c r="C31" t="s">
-        <v>310</v>
+        <v>410</v>
       </c>
       <c r="D31" t="s">
-        <v>358</v>
+        <v>475</v>
       </c>
     </row>
     <row r="32" spans="1:4">
@@ -1905,13 +2259,13 @@
         <v>34</v>
       </c>
       <c r="B32" t="s">
-        <v>182</v>
+        <v>232</v>
       </c>
       <c r="C32" t="s">
-        <v>311</v>
+        <v>411</v>
       </c>
       <c r="D32" t="s">
-        <v>358</v>
+        <v>475</v>
       </c>
     </row>
     <row r="33" spans="1:4">
@@ -1919,13 +2273,13 @@
         <v>35</v>
       </c>
       <c r="B33" t="s">
-        <v>183</v>
+        <v>233</v>
       </c>
       <c r="C33" t="s">
-        <v>311</v>
+        <v>411</v>
       </c>
       <c r="D33" t="s">
-        <v>358</v>
+        <v>475</v>
       </c>
     </row>
     <row r="34" spans="1:4">
@@ -1933,13 +2287,13 @@
         <v>36</v>
       </c>
       <c r="B34" t="s">
-        <v>184</v>
+        <v>234</v>
       </c>
       <c r="C34" t="s">
-        <v>311</v>
+        <v>411</v>
       </c>
       <c r="D34" t="s">
-        <v>358</v>
+        <v>475</v>
       </c>
     </row>
     <row r="35" spans="1:4">
@@ -1947,13 +2301,13 @@
         <v>37</v>
       </c>
       <c r="B35" t="s">
-        <v>185</v>
+        <v>235</v>
       </c>
       <c r="C35" t="s">
-        <v>312</v>
+        <v>412</v>
       </c>
       <c r="D35" t="s">
-        <v>358</v>
+        <v>475</v>
       </c>
     </row>
     <row r="36" spans="1:4">
@@ -1961,13 +2315,13 @@
         <v>38</v>
       </c>
       <c r="B36" t="s">
-        <v>186</v>
+        <v>236</v>
       </c>
       <c r="C36" t="s">
-        <v>312</v>
+        <v>412</v>
       </c>
       <c r="D36" t="s">
-        <v>358</v>
+        <v>475</v>
       </c>
     </row>
     <row r="37" spans="1:4">
@@ -1975,13 +2329,13 @@
         <v>5</v>
       </c>
       <c r="B37" t="s">
-        <v>153</v>
+        <v>203</v>
       </c>
       <c r="C37" t="s">
-        <v>312</v>
+        <v>412</v>
       </c>
       <c r="D37" t="s">
-        <v>358</v>
+        <v>475</v>
       </c>
     </row>
     <row r="38" spans="1:4">
@@ -1989,13 +2343,13 @@
         <v>39</v>
       </c>
       <c r="B38" t="s">
-        <v>187</v>
+        <v>237</v>
       </c>
       <c r="C38" t="s">
-        <v>313</v>
+        <v>413</v>
       </c>
       <c r="D38" t="s">
-        <v>358</v>
+        <v>475</v>
       </c>
     </row>
     <row r="39" spans="1:4">
@@ -2003,13 +2357,13 @@
         <v>40</v>
       </c>
       <c r="B39" t="s">
-        <v>188</v>
+        <v>238</v>
       </c>
       <c r="C39" t="s">
-        <v>313</v>
+        <v>413</v>
       </c>
       <c r="D39" t="s">
-        <v>358</v>
+        <v>475</v>
       </c>
     </row>
     <row r="40" spans="1:4">
@@ -2017,13 +2371,13 @@
         <v>41</v>
       </c>
       <c r="B40" t="s">
-        <v>189</v>
+        <v>239</v>
       </c>
       <c r="C40" t="s">
-        <v>313</v>
+        <v>413</v>
       </c>
       <c r="D40" t="s">
-        <v>358</v>
+        <v>475</v>
       </c>
     </row>
     <row r="41" spans="1:4">
@@ -2031,13 +2385,13 @@
         <v>42</v>
       </c>
       <c r="B41" t="s">
-        <v>190</v>
+        <v>240</v>
       </c>
       <c r="C41" t="s">
-        <v>314</v>
+        <v>414</v>
       </c>
       <c r="D41" t="s">
-        <v>358</v>
+        <v>475</v>
       </c>
     </row>
     <row r="42" spans="1:4">
@@ -2045,13 +2399,13 @@
         <v>43</v>
       </c>
       <c r="B42" t="s">
-        <v>191</v>
+        <v>241</v>
       </c>
       <c r="C42" t="s">
-        <v>314</v>
+        <v>414</v>
       </c>
       <c r="D42" t="s">
-        <v>358</v>
+        <v>475</v>
       </c>
     </row>
     <row r="43" spans="1:4">
@@ -2059,13 +2413,13 @@
         <v>44</v>
       </c>
       <c r="B43" t="s">
-        <v>192</v>
+        <v>242</v>
       </c>
       <c r="C43" t="s">
-        <v>314</v>
+        <v>414</v>
       </c>
       <c r="D43" t="s">
-        <v>358</v>
+        <v>475</v>
       </c>
     </row>
     <row r="44" spans="1:4">
@@ -2073,13 +2427,13 @@
         <v>45</v>
       </c>
       <c r="B44" t="s">
-        <v>193</v>
+        <v>243</v>
       </c>
       <c r="C44" t="s">
-        <v>315</v>
+        <v>415</v>
       </c>
       <c r="D44" t="s">
-        <v>358</v>
+        <v>475</v>
       </c>
     </row>
     <row r="45" spans="1:4">
@@ -2087,13 +2441,13 @@
         <v>46</v>
       </c>
       <c r="B45" t="s">
-        <v>194</v>
+        <v>244</v>
       </c>
       <c r="C45" t="s">
-        <v>315</v>
+        <v>415</v>
       </c>
       <c r="D45" t="s">
-        <v>358</v>
+        <v>475</v>
       </c>
     </row>
     <row r="46" spans="1:4">
@@ -2101,13 +2455,13 @@
         <v>47</v>
       </c>
       <c r="B46" t="s">
-        <v>195</v>
+        <v>245</v>
       </c>
       <c r="C46" t="s">
-        <v>315</v>
+        <v>415</v>
       </c>
       <c r="D46" t="s">
-        <v>358</v>
+        <v>475</v>
       </c>
     </row>
     <row r="47" spans="1:4">
@@ -2115,13 +2469,13 @@
         <v>48</v>
       </c>
       <c r="B47" t="s">
-        <v>196</v>
+        <v>246</v>
       </c>
       <c r="C47" t="s">
-        <v>316</v>
+        <v>416</v>
       </c>
       <c r="D47" t="s">
-        <v>358</v>
+        <v>475</v>
       </c>
     </row>
     <row r="48" spans="1:4">
@@ -2129,13 +2483,13 @@
         <v>49</v>
       </c>
       <c r="B48" t="s">
-        <v>197</v>
+        <v>247</v>
       </c>
       <c r="C48" t="s">
-        <v>316</v>
+        <v>416</v>
       </c>
       <c r="D48" t="s">
-        <v>358</v>
+        <v>475</v>
       </c>
     </row>
     <row r="49" spans="1:4">
@@ -2143,13 +2497,13 @@
         <v>50</v>
       </c>
       <c r="B49" t="s">
-        <v>198</v>
+        <v>248</v>
       </c>
       <c r="C49" t="s">
-        <v>316</v>
+        <v>416</v>
       </c>
       <c r="D49" t="s">
-        <v>358</v>
+        <v>475</v>
       </c>
     </row>
     <row r="50" spans="1:4">
@@ -2157,13 +2511,13 @@
         <v>51</v>
       </c>
       <c r="B50" t="s">
-        <v>199</v>
+        <v>249</v>
       </c>
       <c r="C50" t="s">
-        <v>317</v>
+        <v>417</v>
       </c>
       <c r="D50" t="s">
-        <v>358</v>
+        <v>475</v>
       </c>
     </row>
     <row r="51" spans="1:4">
@@ -2171,13 +2525,13 @@
         <v>52</v>
       </c>
       <c r="B51" t="s">
-        <v>200</v>
+        <v>250</v>
       </c>
       <c r="C51" t="s">
-        <v>318</v>
+        <v>418</v>
       </c>
       <c r="D51" t="s">
-        <v>358</v>
+        <v>475</v>
       </c>
     </row>
     <row r="52" spans="1:4">
@@ -2185,13 +2539,13 @@
         <v>53</v>
       </c>
       <c r="B52" t="s">
-        <v>201</v>
+        <v>251</v>
       </c>
       <c r="C52" t="s">
-        <v>318</v>
+        <v>418</v>
       </c>
       <c r="D52" t="s">
-        <v>358</v>
+        <v>475</v>
       </c>
     </row>
     <row r="53" spans="1:4">
@@ -2199,13 +2553,13 @@
         <v>54</v>
       </c>
       <c r="B53" t="s">
-        <v>202</v>
+        <v>252</v>
       </c>
       <c r="C53" t="s">
-        <v>318</v>
+        <v>418</v>
       </c>
       <c r="D53" t="s">
-        <v>358</v>
+        <v>475</v>
       </c>
     </row>
     <row r="54" spans="1:4">
@@ -2213,13 +2567,13 @@
         <v>55</v>
       </c>
       <c r="B54" t="s">
-        <v>203</v>
+        <v>253</v>
       </c>
       <c r="C54" t="s">
-        <v>319</v>
+        <v>419</v>
       </c>
       <c r="D54" t="s">
-        <v>358</v>
+        <v>475</v>
       </c>
     </row>
     <row r="55" spans="1:4">
@@ -2227,13 +2581,13 @@
         <v>56</v>
       </c>
       <c r="B55" t="s">
-        <v>204</v>
+        <v>254</v>
       </c>
       <c r="C55" t="s">
-        <v>319</v>
+        <v>419</v>
       </c>
       <c r="D55" t="s">
-        <v>358</v>
+        <v>475</v>
       </c>
     </row>
     <row r="56" spans="1:4">
@@ -2241,13 +2595,13 @@
         <v>57</v>
       </c>
       <c r="B56" t="s">
-        <v>205</v>
+        <v>255</v>
       </c>
       <c r="C56" t="s">
-        <v>319</v>
+        <v>419</v>
       </c>
       <c r="D56" t="s">
-        <v>358</v>
+        <v>475</v>
       </c>
     </row>
     <row r="57" spans="1:4">
@@ -2255,13 +2609,13 @@
         <v>58</v>
       </c>
       <c r="B57" t="s">
-        <v>206</v>
+        <v>256</v>
       </c>
       <c r="C57" t="s">
-        <v>320</v>
+        <v>420</v>
       </c>
       <c r="D57" t="s">
-        <v>358</v>
+        <v>475</v>
       </c>
     </row>
     <row r="58" spans="1:4">
@@ -2269,13 +2623,13 @@
         <v>59</v>
       </c>
       <c r="B58" t="s">
-        <v>207</v>
+        <v>257</v>
       </c>
       <c r="C58" t="s">
-        <v>321</v>
+        <v>421</v>
       </c>
       <c r="D58" t="s">
-        <v>358</v>
+        <v>475</v>
       </c>
     </row>
     <row r="59" spans="1:4">
@@ -2283,13 +2637,13 @@
         <v>60</v>
       </c>
       <c r="B59" t="s">
-        <v>208</v>
+        <v>258</v>
       </c>
       <c r="C59" t="s">
-        <v>321</v>
+        <v>421</v>
       </c>
       <c r="D59" t="s">
-        <v>358</v>
+        <v>475</v>
       </c>
     </row>
     <row r="60" spans="1:4">
@@ -2297,13 +2651,13 @@
         <v>61</v>
       </c>
       <c r="B60" t="s">
-        <v>209</v>
+        <v>259</v>
       </c>
       <c r="C60" t="s">
-        <v>321</v>
+        <v>421</v>
       </c>
       <c r="D60" t="s">
-        <v>358</v>
+        <v>475</v>
       </c>
     </row>
     <row r="61" spans="1:4">
@@ -2311,13 +2665,13 @@
         <v>62</v>
       </c>
       <c r="B61" t="s">
-        <v>210</v>
+        <v>260</v>
       </c>
       <c r="C61" t="s">
-        <v>322</v>
+        <v>422</v>
       </c>
       <c r="D61" t="s">
-        <v>358</v>
+        <v>475</v>
       </c>
     </row>
     <row r="62" spans="1:4">
@@ -2325,13 +2679,13 @@
         <v>63</v>
       </c>
       <c r="B62" t="s">
-        <v>211</v>
+        <v>261</v>
       </c>
       <c r="C62" t="s">
-        <v>322</v>
+        <v>422</v>
       </c>
       <c r="D62" t="s">
-        <v>358</v>
+        <v>475</v>
       </c>
     </row>
     <row r="63" spans="1:4">
@@ -2339,13 +2693,13 @@
         <v>64</v>
       </c>
       <c r="B63" t="s">
-        <v>212</v>
+        <v>262</v>
       </c>
       <c r="C63" t="s">
-        <v>322</v>
+        <v>422</v>
       </c>
       <c r="D63" t="s">
-        <v>358</v>
+        <v>475</v>
       </c>
     </row>
     <row r="64" spans="1:4">
@@ -2353,13 +2707,13 @@
         <v>65</v>
       </c>
       <c r="B64" t="s">
-        <v>213</v>
+        <v>263</v>
       </c>
       <c r="C64" t="s">
-        <v>323</v>
+        <v>423</v>
       </c>
       <c r="D64" t="s">
-        <v>358</v>
+        <v>475</v>
       </c>
     </row>
     <row r="65" spans="1:4">
@@ -2367,13 +2721,13 @@
         <v>66</v>
       </c>
       <c r="B65" t="s">
-        <v>214</v>
+        <v>264</v>
       </c>
       <c r="C65" t="s">
-        <v>323</v>
+        <v>423</v>
       </c>
       <c r="D65" t="s">
-        <v>358</v>
+        <v>475</v>
       </c>
     </row>
     <row r="66" spans="1:4">
@@ -2381,13 +2735,13 @@
         <v>67</v>
       </c>
       <c r="B66" t="s">
-        <v>215</v>
+        <v>265</v>
       </c>
       <c r="C66" t="s">
-        <v>323</v>
+        <v>423</v>
       </c>
       <c r="D66" t="s">
-        <v>358</v>
+        <v>475</v>
       </c>
     </row>
     <row r="67" spans="1:4">
@@ -2395,13 +2749,13 @@
         <v>68</v>
       </c>
       <c r="B67" t="s">
-        <v>216</v>
+        <v>266</v>
       </c>
       <c r="C67" t="s">
-        <v>324</v>
+        <v>424</v>
       </c>
       <c r="D67" t="s">
-        <v>358</v>
+        <v>475</v>
       </c>
     </row>
     <row r="68" spans="1:4">
@@ -2409,13 +2763,13 @@
         <v>69</v>
       </c>
       <c r="B68" t="s">
-        <v>217</v>
+        <v>267</v>
       </c>
       <c r="C68" t="s">
-        <v>324</v>
+        <v>424</v>
       </c>
       <c r="D68" t="s">
-        <v>358</v>
+        <v>475</v>
       </c>
     </row>
     <row r="69" spans="1:4">
@@ -2423,13 +2777,13 @@
         <v>70</v>
       </c>
       <c r="B69" t="s">
-        <v>218</v>
+        <v>268</v>
       </c>
       <c r="C69" t="s">
-        <v>324</v>
+        <v>424</v>
       </c>
       <c r="D69" t="s">
-        <v>358</v>
+        <v>475</v>
       </c>
     </row>
     <row r="70" spans="1:4">
@@ -2437,13 +2791,13 @@
         <v>71</v>
       </c>
       <c r="B70" t="s">
-        <v>219</v>
+        <v>269</v>
       </c>
       <c r="C70" t="s">
-        <v>325</v>
+        <v>425</v>
       </c>
       <c r="D70" t="s">
-        <v>359</v>
+        <v>476</v>
       </c>
     </row>
     <row r="71" spans="1:4">
@@ -2451,13 +2805,13 @@
         <v>72</v>
       </c>
       <c r="B71" t="s">
-        <v>220</v>
+        <v>270</v>
       </c>
       <c r="C71" t="s">
-        <v>325</v>
+        <v>425</v>
       </c>
       <c r="D71" t="s">
-        <v>359</v>
+        <v>476</v>
       </c>
     </row>
     <row r="72" spans="1:4">
@@ -2465,13 +2819,13 @@
         <v>73</v>
       </c>
       <c r="B72" t="s">
-        <v>221</v>
+        <v>271</v>
       </c>
       <c r="C72" t="s">
-        <v>325</v>
+        <v>425</v>
       </c>
       <c r="D72" t="s">
-        <v>359</v>
+        <v>476</v>
       </c>
     </row>
     <row r="73" spans="1:4">
@@ -2479,13 +2833,13 @@
         <v>74</v>
       </c>
       <c r="B73" t="s">
-        <v>222</v>
+        <v>272</v>
       </c>
       <c r="C73" t="s">
-        <v>326</v>
+        <v>426</v>
       </c>
       <c r="D73" t="s">
-        <v>359</v>
+        <v>476</v>
       </c>
     </row>
     <row r="74" spans="1:4">
@@ -2493,13 +2847,13 @@
         <v>75</v>
       </c>
       <c r="B74" t="s">
-        <v>223</v>
+        <v>273</v>
       </c>
       <c r="C74" t="s">
-        <v>326</v>
+        <v>426</v>
       </c>
       <c r="D74" t="s">
-        <v>359</v>
+        <v>476</v>
       </c>
     </row>
     <row r="75" spans="1:4">
@@ -2507,13 +2861,13 @@
         <v>76</v>
       </c>
       <c r="B75" t="s">
-        <v>224</v>
+        <v>274</v>
       </c>
       <c r="C75" t="s">
-        <v>326</v>
+        <v>426</v>
       </c>
       <c r="D75" t="s">
-        <v>359</v>
+        <v>476</v>
       </c>
     </row>
     <row r="76" spans="1:4">
@@ -2521,13 +2875,13 @@
         <v>77</v>
       </c>
       <c r="B76" t="s">
-        <v>225</v>
+        <v>275</v>
       </c>
       <c r="C76" t="s">
-        <v>327</v>
+        <v>427</v>
       </c>
       <c r="D76" t="s">
-        <v>359</v>
+        <v>476</v>
       </c>
     </row>
     <row r="77" spans="1:4">
@@ -2535,13 +2889,13 @@
         <v>78</v>
       </c>
       <c r="B77" t="s">
-        <v>226</v>
+        <v>276</v>
       </c>
       <c r="C77" t="s">
-        <v>327</v>
+        <v>427</v>
       </c>
       <c r="D77" t="s">
-        <v>359</v>
+        <v>476</v>
       </c>
     </row>
     <row r="78" spans="1:4">
@@ -2549,13 +2903,13 @@
         <v>79</v>
       </c>
       <c r="B78" t="s">
-        <v>227</v>
+        <v>277</v>
       </c>
       <c r="C78" t="s">
-        <v>327</v>
+        <v>427</v>
       </c>
       <c r="D78" t="s">
-        <v>359</v>
+        <v>476</v>
       </c>
     </row>
     <row r="79" spans="1:4">
@@ -2563,13 +2917,13 @@
         <v>78</v>
       </c>
       <c r="B79" t="s">
-        <v>226</v>
+        <v>276</v>
       </c>
       <c r="C79" t="s">
-        <v>328</v>
+        <v>428</v>
       </c>
       <c r="D79" t="s">
-        <v>359</v>
+        <v>476</v>
       </c>
     </row>
     <row r="80" spans="1:4">
@@ -2577,13 +2931,13 @@
         <v>80</v>
       </c>
       <c r="B80" t="s">
-        <v>228</v>
+        <v>278</v>
       </c>
       <c r="C80" t="s">
-        <v>328</v>
+        <v>428</v>
       </c>
       <c r="D80" t="s">
-        <v>359</v>
+        <v>476</v>
       </c>
     </row>
     <row r="81" spans="1:4">
@@ -2591,13 +2945,13 @@
         <v>81</v>
       </c>
       <c r="B81" t="s">
-        <v>229</v>
+        <v>279</v>
       </c>
       <c r="C81" t="s">
-        <v>328</v>
+        <v>428</v>
       </c>
       <c r="D81" t="s">
-        <v>359</v>
+        <v>476</v>
       </c>
     </row>
     <row r="82" spans="1:4">
@@ -2605,13 +2959,13 @@
         <v>10</v>
       </c>
       <c r="B82" t="s">
-        <v>158</v>
+        <v>208</v>
       </c>
       <c r="C82" t="s">
-        <v>329</v>
+        <v>429</v>
       </c>
       <c r="D82" t="s">
-        <v>359</v>
+        <v>476</v>
       </c>
     </row>
     <row r="83" spans="1:4">
@@ -2619,13 +2973,13 @@
         <v>82</v>
       </c>
       <c r="B83" t="s">
-        <v>230</v>
+        <v>280</v>
       </c>
       <c r="C83" t="s">
-        <v>329</v>
+        <v>429</v>
       </c>
       <c r="D83" t="s">
-        <v>359</v>
+        <v>476</v>
       </c>
     </row>
     <row r="84" spans="1:4">
@@ -2633,13 +2987,13 @@
         <v>83</v>
       </c>
       <c r="B84" t="s">
-        <v>231</v>
+        <v>281</v>
       </c>
       <c r="C84" t="s">
-        <v>329</v>
+        <v>429</v>
       </c>
       <c r="D84" t="s">
-        <v>359</v>
+        <v>476</v>
       </c>
     </row>
     <row r="85" spans="1:4">
@@ -2647,13 +3001,13 @@
         <v>10</v>
       </c>
       <c r="B85" t="s">
-        <v>158</v>
+        <v>208</v>
       </c>
       <c r="C85" t="s">
-        <v>330</v>
+        <v>430</v>
       </c>
       <c r="D85" t="s">
-        <v>359</v>
+        <v>476</v>
       </c>
     </row>
     <row r="86" spans="1:4">
@@ -2661,13 +3015,13 @@
         <v>84</v>
       </c>
       <c r="B86" t="s">
-        <v>232</v>
+        <v>282</v>
       </c>
       <c r="C86" t="s">
-        <v>330</v>
+        <v>430</v>
       </c>
       <c r="D86" t="s">
-        <v>359</v>
+        <v>476</v>
       </c>
     </row>
     <row r="87" spans="1:4">
@@ -2675,13 +3029,13 @@
         <v>85</v>
       </c>
       <c r="B87" t="s">
-        <v>233</v>
+        <v>283</v>
       </c>
       <c r="C87" t="s">
-        <v>330</v>
+        <v>430</v>
       </c>
       <c r="D87" t="s">
-        <v>359</v>
+        <v>476</v>
       </c>
     </row>
     <row r="88" spans="1:4">
@@ -2689,13 +3043,13 @@
         <v>11</v>
       </c>
       <c r="B88" t="s">
-        <v>159</v>
+        <v>209</v>
       </c>
       <c r="C88" t="s">
-        <v>331</v>
+        <v>431</v>
       </c>
       <c r="D88" t="s">
-        <v>359</v>
+        <v>476</v>
       </c>
     </row>
     <row r="89" spans="1:4">
@@ -2703,13 +3057,13 @@
         <v>86</v>
       </c>
       <c r="B89" t="s">
-        <v>234</v>
+        <v>284</v>
       </c>
       <c r="C89" t="s">
-        <v>331</v>
+        <v>431</v>
       </c>
       <c r="D89" t="s">
-        <v>359</v>
+        <v>476</v>
       </c>
     </row>
     <row r="90" spans="1:4">
@@ -2717,13 +3071,13 @@
         <v>87</v>
       </c>
       <c r="B90" t="s">
-        <v>235</v>
+        <v>285</v>
       </c>
       <c r="C90" t="s">
-        <v>331</v>
+        <v>431</v>
       </c>
       <c r="D90" t="s">
-        <v>359</v>
+        <v>476</v>
       </c>
     </row>
     <row r="91" spans="1:4">
@@ -2731,13 +3085,13 @@
         <v>88</v>
       </c>
       <c r="B91" t="s">
-        <v>236</v>
+        <v>286</v>
       </c>
       <c r="C91" t="s">
-        <v>332</v>
+        <v>432</v>
       </c>
       <c r="D91" t="s">
-        <v>360</v>
+        <v>477</v>
       </c>
     </row>
     <row r="92" spans="1:4">
@@ -2745,13 +3099,13 @@
         <v>89</v>
       </c>
       <c r="B92" t="s">
-        <v>237</v>
+        <v>287</v>
       </c>
       <c r="C92" t="s">
-        <v>332</v>
+        <v>432</v>
       </c>
       <c r="D92" t="s">
-        <v>360</v>
+        <v>477</v>
       </c>
     </row>
     <row r="93" spans="1:4">
@@ -2759,13 +3113,13 @@
         <v>90</v>
       </c>
       <c r="B93" t="s">
-        <v>238</v>
+        <v>288</v>
       </c>
       <c r="C93" t="s">
-        <v>332</v>
+        <v>432</v>
       </c>
       <c r="D93" t="s">
-        <v>360</v>
+        <v>477</v>
       </c>
     </row>
     <row r="94" spans="1:4">
@@ -2773,13 +3127,13 @@
         <v>91</v>
       </c>
       <c r="B94" t="s">
-        <v>239</v>
+        <v>289</v>
       </c>
       <c r="C94" t="s">
-        <v>333</v>
+        <v>433</v>
       </c>
       <c r="D94" t="s">
-        <v>360</v>
+        <v>477</v>
       </c>
     </row>
     <row r="95" spans="1:4">
@@ -2787,13 +3141,13 @@
         <v>92</v>
       </c>
       <c r="B95" t="s">
-        <v>240</v>
+        <v>290</v>
       </c>
       <c r="C95" t="s">
-        <v>333</v>
+        <v>433</v>
       </c>
       <c r="D95" t="s">
-        <v>360</v>
+        <v>477</v>
       </c>
     </row>
     <row r="96" spans="1:4">
@@ -2801,13 +3155,13 @@
         <v>93</v>
       </c>
       <c r="B96" t="s">
-        <v>241</v>
+        <v>291</v>
       </c>
       <c r="C96" t="s">
-        <v>333</v>
+        <v>433</v>
       </c>
       <c r="D96" t="s">
-        <v>360</v>
+        <v>477</v>
       </c>
     </row>
     <row r="97" spans="1:4">
@@ -2815,13 +3169,13 @@
         <v>12</v>
       </c>
       <c r="B97" t="s">
-        <v>160</v>
+        <v>210</v>
       </c>
       <c r="C97" t="s">
-        <v>334</v>
+        <v>434</v>
       </c>
       <c r="D97" t="s">
-        <v>360</v>
+        <v>477</v>
       </c>
     </row>
     <row r="98" spans="1:4">
@@ -2829,13 +3183,13 @@
         <v>94</v>
       </c>
       <c r="B98" t="s">
-        <v>242</v>
+        <v>292</v>
       </c>
       <c r="C98" t="s">
-        <v>335</v>
+        <v>435</v>
       </c>
       <c r="D98" t="s">
-        <v>360</v>
+        <v>477</v>
       </c>
     </row>
     <row r="99" spans="1:4">
@@ -2843,13 +3197,13 @@
         <v>95</v>
       </c>
       <c r="B99" t="s">
-        <v>243</v>
+        <v>293</v>
       </c>
       <c r="C99" t="s">
-        <v>335</v>
+        <v>435</v>
       </c>
       <c r="D99" t="s">
-        <v>360</v>
+        <v>477</v>
       </c>
     </row>
     <row r="100" spans="1:4">
@@ -2857,13 +3211,13 @@
         <v>96</v>
       </c>
       <c r="B100" t="s">
-        <v>244</v>
+        <v>294</v>
       </c>
       <c r="C100" t="s">
-        <v>335</v>
+        <v>435</v>
       </c>
       <c r="D100" t="s">
-        <v>360</v>
+        <v>477</v>
       </c>
     </row>
     <row r="101" spans="1:4">
@@ -2871,13 +3225,13 @@
         <v>97</v>
       </c>
       <c r="B101" t="s">
-        <v>245</v>
+        <v>295</v>
       </c>
       <c r="C101" t="s">
-        <v>336</v>
+        <v>436</v>
       </c>
       <c r="D101" t="s">
-        <v>360</v>
+        <v>477</v>
       </c>
     </row>
     <row r="102" spans="1:4">
@@ -2885,13 +3239,13 @@
         <v>98</v>
       </c>
       <c r="B102" t="s">
-        <v>246</v>
+        <v>296</v>
       </c>
       <c r="C102" t="s">
-        <v>336</v>
+        <v>436</v>
       </c>
       <c r="D102" t="s">
-        <v>360</v>
+        <v>477</v>
       </c>
     </row>
     <row r="103" spans="1:4">
@@ -2899,13 +3253,13 @@
         <v>99</v>
       </c>
       <c r="B103" t="s">
-        <v>247</v>
+        <v>297</v>
       </c>
       <c r="C103" t="s">
-        <v>336</v>
+        <v>436</v>
       </c>
       <c r="D103" t="s">
-        <v>360</v>
+        <v>477</v>
       </c>
     </row>
     <row r="104" spans="1:4">
@@ -2913,13 +3267,13 @@
         <v>100</v>
       </c>
       <c r="B104" t="s">
-        <v>248</v>
+        <v>298</v>
       </c>
       <c r="C104" t="s">
-        <v>337</v>
+        <v>437</v>
       </c>
       <c r="D104" t="s">
-        <v>360</v>
+        <v>477</v>
       </c>
     </row>
     <row r="105" spans="1:4">
@@ -2927,13 +3281,13 @@
         <v>101</v>
       </c>
       <c r="B105" t="s">
-        <v>249</v>
+        <v>299</v>
       </c>
       <c r="C105" t="s">
-        <v>337</v>
+        <v>437</v>
       </c>
       <c r="D105" t="s">
-        <v>360</v>
+        <v>477</v>
       </c>
     </row>
     <row r="106" spans="1:4">
@@ -2941,13 +3295,13 @@
         <v>102</v>
       </c>
       <c r="B106" t="s">
-        <v>250</v>
+        <v>300</v>
       </c>
       <c r="C106" t="s">
-        <v>337</v>
+        <v>437</v>
       </c>
       <c r="D106" t="s">
-        <v>360</v>
+        <v>477</v>
       </c>
     </row>
     <row r="107" spans="1:4">
@@ -2955,13 +3309,13 @@
         <v>103</v>
       </c>
       <c r="B107" t="s">
-        <v>251</v>
+        <v>301</v>
       </c>
       <c r="C107" t="s">
-        <v>338</v>
+        <v>438</v>
       </c>
       <c r="D107" t="s">
-        <v>360</v>
+        <v>477</v>
       </c>
     </row>
     <row r="108" spans="1:4">
@@ -2969,13 +3323,13 @@
         <v>104</v>
       </c>
       <c r="B108" t="s">
-        <v>252</v>
+        <v>302</v>
       </c>
       <c r="C108" t="s">
-        <v>338</v>
+        <v>438</v>
       </c>
       <c r="D108" t="s">
-        <v>360</v>
+        <v>477</v>
       </c>
     </row>
     <row r="109" spans="1:4">
@@ -2983,13 +3337,13 @@
         <v>105</v>
       </c>
       <c r="B109" t="s">
-        <v>253</v>
+        <v>303</v>
       </c>
       <c r="C109" t="s">
-        <v>338</v>
+        <v>438</v>
       </c>
       <c r="D109" t="s">
-        <v>360</v>
+        <v>477</v>
       </c>
     </row>
     <row r="110" spans="1:4">
@@ -2997,13 +3351,13 @@
         <v>16</v>
       </c>
       <c r="B110" t="s">
-        <v>164</v>
+        <v>214</v>
       </c>
       <c r="C110" t="s">
-        <v>339</v>
+        <v>439</v>
       </c>
       <c r="D110" t="s">
-        <v>360</v>
+        <v>477</v>
       </c>
     </row>
     <row r="111" spans="1:4">
@@ -3011,13 +3365,13 @@
         <v>106</v>
       </c>
       <c r="B111" t="s">
-        <v>254</v>
+        <v>304</v>
       </c>
       <c r="C111" t="s">
-        <v>339</v>
+        <v>439</v>
       </c>
       <c r="D111" t="s">
-        <v>360</v>
+        <v>477</v>
       </c>
     </row>
     <row r="112" spans="1:4">
@@ -3025,13 +3379,13 @@
         <v>107</v>
       </c>
       <c r="B112" t="s">
-        <v>255</v>
+        <v>305</v>
       </c>
       <c r="C112" t="s">
-        <v>339</v>
+        <v>439</v>
       </c>
       <c r="D112" t="s">
-        <v>360</v>
+        <v>477</v>
       </c>
     </row>
     <row r="113" spans="1:4">
@@ -3039,13 +3393,13 @@
         <v>16</v>
       </c>
       <c r="B113" t="s">
-        <v>164</v>
+        <v>214</v>
       </c>
       <c r="C113" t="s">
-        <v>340</v>
+        <v>440</v>
       </c>
       <c r="D113" t="s">
-        <v>360</v>
+        <v>477</v>
       </c>
     </row>
     <row r="114" spans="1:4">
@@ -3053,13 +3407,13 @@
         <v>108</v>
       </c>
       <c r="B114" t="s">
-        <v>256</v>
+        <v>306</v>
       </c>
       <c r="C114" t="s">
-        <v>340</v>
+        <v>440</v>
       </c>
       <c r="D114" t="s">
-        <v>360</v>
+        <v>477</v>
       </c>
     </row>
     <row r="115" spans="1:4">
@@ -3067,13 +3421,13 @@
         <v>109</v>
       </c>
       <c r="B115" t="s">
-        <v>257</v>
+        <v>307</v>
       </c>
       <c r="C115" t="s">
-        <v>340</v>
+        <v>440</v>
       </c>
       <c r="D115" t="s">
-        <v>360</v>
+        <v>477</v>
       </c>
     </row>
     <row r="116" spans="1:4">
@@ -3081,13 +3435,13 @@
         <v>18</v>
       </c>
       <c r="B116" t="s">
-        <v>166</v>
+        <v>216</v>
       </c>
       <c r="C116" t="s">
-        <v>341</v>
+        <v>441</v>
       </c>
       <c r="D116" t="s">
-        <v>360</v>
+        <v>477</v>
       </c>
     </row>
     <row r="117" spans="1:4">
@@ -3095,13 +3449,13 @@
         <v>110</v>
       </c>
       <c r="B117" t="s">
-        <v>258</v>
+        <v>308</v>
       </c>
       <c r="C117" t="s">
-        <v>341</v>
+        <v>441</v>
       </c>
       <c r="D117" t="s">
-        <v>360</v>
+        <v>477</v>
       </c>
     </row>
     <row r="118" spans="1:4">
@@ -3109,13 +3463,13 @@
         <v>111</v>
       </c>
       <c r="B118" t="s">
-        <v>259</v>
+        <v>309</v>
       </c>
       <c r="C118" t="s">
-        <v>341</v>
+        <v>441</v>
       </c>
       <c r="D118" t="s">
-        <v>360</v>
+        <v>477</v>
       </c>
     </row>
     <row r="119" spans="1:4">
@@ -3123,13 +3477,13 @@
         <v>18</v>
       </c>
       <c r="B119" t="s">
-        <v>166</v>
+        <v>216</v>
       </c>
       <c r="C119" t="s">
-        <v>342</v>
+        <v>442</v>
       </c>
       <c r="D119" t="s">
-        <v>360</v>
+        <v>477</v>
       </c>
     </row>
     <row r="120" spans="1:4">
@@ -3137,13 +3491,13 @@
         <v>112</v>
       </c>
       <c r="B120" t="s">
-        <v>260</v>
+        <v>310</v>
       </c>
       <c r="C120" t="s">
-        <v>342</v>
+        <v>442</v>
       </c>
       <c r="D120" t="s">
-        <v>360</v>
+        <v>477</v>
       </c>
     </row>
     <row r="121" spans="1:4">
@@ -3151,13 +3505,13 @@
         <v>113</v>
       </c>
       <c r="B121" t="s">
-        <v>261</v>
+        <v>311</v>
       </c>
       <c r="C121" t="s">
-        <v>342</v>
+        <v>442</v>
       </c>
       <c r="D121" t="s">
-        <v>360</v>
+        <v>477</v>
       </c>
     </row>
     <row r="122" spans="1:4">
@@ -3165,13 +3519,13 @@
         <v>114</v>
       </c>
       <c r="B122" t="s">
-        <v>262</v>
+        <v>312</v>
       </c>
       <c r="C122" t="s">
-        <v>343</v>
+        <v>443</v>
       </c>
       <c r="D122" t="s">
-        <v>361</v>
+        <v>478</v>
       </c>
     </row>
     <row r="123" spans="1:4">
@@ -3179,13 +3533,13 @@
         <v>19</v>
       </c>
       <c r="B123" t="s">
-        <v>167</v>
+        <v>217</v>
       </c>
       <c r="C123" t="s">
-        <v>343</v>
+        <v>443</v>
       </c>
       <c r="D123" t="s">
-        <v>361</v>
+        <v>478</v>
       </c>
     </row>
     <row r="124" spans="1:4">
@@ -3193,13 +3547,13 @@
         <v>115</v>
       </c>
       <c r="B124" t="s">
-        <v>263</v>
+        <v>313</v>
       </c>
       <c r="C124" t="s">
-        <v>343</v>
+        <v>443</v>
       </c>
       <c r="D124" t="s">
-        <v>361</v>
+        <v>478</v>
       </c>
     </row>
     <row r="125" spans="1:4">
@@ -3207,13 +3561,13 @@
         <v>116</v>
       </c>
       <c r="B125" t="s">
-        <v>264</v>
+        <v>314</v>
       </c>
       <c r="C125" t="s">
-        <v>344</v>
+        <v>444</v>
       </c>
       <c r="D125" t="s">
-        <v>361</v>
+        <v>478</v>
       </c>
     </row>
     <row r="126" spans="1:4">
@@ -3221,13 +3575,13 @@
         <v>117</v>
       </c>
       <c r="B126" t="s">
-        <v>265</v>
+        <v>315</v>
       </c>
       <c r="C126" t="s">
-        <v>344</v>
+        <v>444</v>
       </c>
       <c r="D126" t="s">
-        <v>361</v>
+        <v>478</v>
       </c>
     </row>
     <row r="127" spans="1:4">
@@ -3235,13 +3589,13 @@
         <v>118</v>
       </c>
       <c r="B127" t="s">
-        <v>266</v>
+        <v>316</v>
       </c>
       <c r="C127" t="s">
-        <v>344</v>
+        <v>444</v>
       </c>
       <c r="D127" t="s">
-        <v>361</v>
+        <v>478</v>
       </c>
     </row>
     <row r="128" spans="1:4">
@@ -3249,13 +3603,13 @@
         <v>20</v>
       </c>
       <c r="B128" t="s">
-        <v>168</v>
+        <v>218</v>
       </c>
       <c r="C128" t="s">
-        <v>345</v>
+        <v>445</v>
       </c>
       <c r="D128" t="s">
-        <v>361</v>
+        <v>478</v>
       </c>
     </row>
     <row r="129" spans="1:4">
@@ -3263,13 +3617,13 @@
         <v>119</v>
       </c>
       <c r="B129" t="s">
-        <v>267</v>
+        <v>317</v>
       </c>
       <c r="C129" t="s">
-        <v>345</v>
+        <v>445</v>
       </c>
       <c r="D129" t="s">
-        <v>361</v>
+        <v>478</v>
       </c>
     </row>
     <row r="130" spans="1:4">
@@ -3277,13 +3631,13 @@
         <v>120</v>
       </c>
       <c r="B130" t="s">
-        <v>268</v>
+        <v>318</v>
       </c>
       <c r="C130" t="s">
-        <v>345</v>
+        <v>445</v>
       </c>
       <c r="D130" t="s">
-        <v>361</v>
+        <v>478</v>
       </c>
     </row>
     <row r="131" spans="1:4">
@@ -3291,13 +3645,13 @@
         <v>121</v>
       </c>
       <c r="B131" t="s">
-        <v>269</v>
+        <v>319</v>
       </c>
       <c r="C131" t="s">
-        <v>346</v>
+        <v>446</v>
       </c>
       <c r="D131" t="s">
-        <v>361</v>
+        <v>478</v>
       </c>
     </row>
     <row r="132" spans="1:4">
@@ -3305,13 +3659,13 @@
         <v>122</v>
       </c>
       <c r="B132" t="s">
-        <v>270</v>
+        <v>320</v>
       </c>
       <c r="C132" t="s">
-        <v>346</v>
+        <v>446</v>
       </c>
       <c r="D132" t="s">
-        <v>361</v>
+        <v>478</v>
       </c>
     </row>
     <row r="133" spans="1:4">
@@ -3319,13 +3673,13 @@
         <v>123</v>
       </c>
       <c r="B133" t="s">
-        <v>271</v>
+        <v>321</v>
       </c>
       <c r="C133" t="s">
-        <v>346</v>
+        <v>446</v>
       </c>
       <c r="D133" t="s">
-        <v>361</v>
+        <v>478</v>
       </c>
     </row>
     <row r="134" spans="1:4">
@@ -3333,13 +3687,13 @@
         <v>124</v>
       </c>
       <c r="B134" t="s">
-        <v>272</v>
+        <v>322</v>
       </c>
       <c r="C134" t="s">
-        <v>347</v>
+        <v>447</v>
       </c>
       <c r="D134" t="s">
-        <v>361</v>
+        <v>478</v>
       </c>
     </row>
     <row r="135" spans="1:4">
@@ -3347,13 +3701,13 @@
         <v>125</v>
       </c>
       <c r="B135" t="s">
-        <v>273</v>
+        <v>323</v>
       </c>
       <c r="C135" t="s">
-        <v>347</v>
+        <v>447</v>
       </c>
       <c r="D135" t="s">
-        <v>361</v>
+        <v>478</v>
       </c>
     </row>
     <row r="136" spans="1:4">
@@ -3361,13 +3715,13 @@
         <v>126</v>
       </c>
       <c r="B136" t="s">
-        <v>274</v>
+        <v>324</v>
       </c>
       <c r="C136" t="s">
-        <v>347</v>
+        <v>447</v>
       </c>
       <c r="D136" t="s">
-        <v>361</v>
+        <v>478</v>
       </c>
     </row>
     <row r="137" spans="1:4">
@@ -3375,13 +3729,13 @@
         <v>127</v>
       </c>
       <c r="B137" t="s">
-        <v>275</v>
+        <v>325</v>
       </c>
       <c r="C137" t="s">
-        <v>348</v>
+        <v>448</v>
       </c>
       <c r="D137" t="s">
-        <v>362</v>
+        <v>479</v>
       </c>
     </row>
     <row r="138" spans="1:4">
@@ -3389,13 +3743,13 @@
         <v>128</v>
       </c>
       <c r="B138" t="s">
-        <v>276</v>
+        <v>326</v>
       </c>
       <c r="C138" t="s">
-        <v>348</v>
+        <v>448</v>
       </c>
       <c r="D138" t="s">
-        <v>362</v>
+        <v>479</v>
       </c>
     </row>
     <row r="139" spans="1:4">
@@ -3403,13 +3757,13 @@
         <v>129</v>
       </c>
       <c r="B139" t="s">
-        <v>277</v>
+        <v>327</v>
       </c>
       <c r="C139" t="s">
-        <v>348</v>
+        <v>448</v>
       </c>
       <c r="D139" t="s">
-        <v>362</v>
+        <v>479</v>
       </c>
     </row>
     <row r="140" spans="1:4">
@@ -3417,13 +3771,13 @@
         <v>130</v>
       </c>
       <c r="B140" t="s">
-        <v>278</v>
+        <v>328</v>
       </c>
       <c r="C140" t="s">
-        <v>349</v>
+        <v>449</v>
       </c>
       <c r="D140" t="s">
-        <v>362</v>
+        <v>479</v>
       </c>
     </row>
     <row r="141" spans="1:4">
@@ -3431,13 +3785,13 @@
         <v>131</v>
       </c>
       <c r="B141" t="s">
-        <v>279</v>
+        <v>329</v>
       </c>
       <c r="C141" t="s">
-        <v>349</v>
+        <v>449</v>
       </c>
       <c r="D141" t="s">
-        <v>362</v>
+        <v>479</v>
       </c>
     </row>
     <row r="142" spans="1:4">
@@ -3445,13 +3799,13 @@
         <v>132</v>
       </c>
       <c r="B142" t="s">
-        <v>280</v>
+        <v>330</v>
       </c>
       <c r="C142" t="s">
-        <v>349</v>
+        <v>449</v>
       </c>
       <c r="D142" t="s">
-        <v>362</v>
+        <v>479</v>
       </c>
     </row>
     <row r="143" spans="1:4">
@@ -3459,13 +3813,13 @@
         <v>133</v>
       </c>
       <c r="B143" t="s">
-        <v>281</v>
+        <v>331</v>
       </c>
       <c r="C143" t="s">
-        <v>350</v>
+        <v>450</v>
       </c>
       <c r="D143" t="s">
-        <v>362</v>
+        <v>479</v>
       </c>
     </row>
     <row r="144" spans="1:4">
@@ -3473,13 +3827,13 @@
         <v>134</v>
       </c>
       <c r="B144" t="s">
-        <v>282</v>
+        <v>332</v>
       </c>
       <c r="C144" t="s">
-        <v>350</v>
+        <v>450</v>
       </c>
       <c r="D144" t="s">
-        <v>362</v>
+        <v>479</v>
       </c>
     </row>
     <row r="145" spans="1:4">
@@ -3487,13 +3841,13 @@
         <v>135</v>
       </c>
       <c r="B145" t="s">
-        <v>283</v>
+        <v>333</v>
       </c>
       <c r="C145" t="s">
-        <v>350</v>
+        <v>450</v>
       </c>
       <c r="D145" t="s">
-        <v>362</v>
+        <v>479</v>
       </c>
     </row>
     <row r="146" spans="1:4">
@@ -3501,13 +3855,13 @@
         <v>136</v>
       </c>
       <c r="B146" t="s">
-        <v>284</v>
+        <v>334</v>
       </c>
       <c r="C146" t="s">
-        <v>351</v>
+        <v>451</v>
       </c>
       <c r="D146" t="s">
-        <v>362</v>
+        <v>479</v>
       </c>
     </row>
     <row r="147" spans="1:4">
@@ -3515,13 +3869,13 @@
         <v>137</v>
       </c>
       <c r="B147" t="s">
-        <v>285</v>
+        <v>335</v>
       </c>
       <c r="C147" t="s">
-        <v>351</v>
+        <v>451</v>
       </c>
       <c r="D147" t="s">
-        <v>362</v>
+        <v>479</v>
       </c>
     </row>
     <row r="148" spans="1:4">
@@ -3529,13 +3883,13 @@
         <v>138</v>
       </c>
       <c r="B148" t="s">
-        <v>286</v>
+        <v>336</v>
       </c>
       <c r="C148" t="s">
-        <v>351</v>
+        <v>451</v>
       </c>
       <c r="D148" t="s">
-        <v>362</v>
+        <v>479</v>
       </c>
     </row>
     <row r="149" spans="1:4">
@@ -3543,13 +3897,13 @@
         <v>139</v>
       </c>
       <c r="B149" t="s">
-        <v>287</v>
+        <v>337</v>
       </c>
       <c r="C149" t="s">
-        <v>352</v>
+        <v>452</v>
       </c>
       <c r="D149" t="s">
-        <v>362</v>
+        <v>479</v>
       </c>
     </row>
     <row r="150" spans="1:4">
@@ -3557,13 +3911,13 @@
         <v>140</v>
       </c>
       <c r="B150" t="s">
-        <v>288</v>
+        <v>338</v>
       </c>
       <c r="C150" t="s">
-        <v>352</v>
+        <v>452</v>
       </c>
       <c r="D150" t="s">
-        <v>362</v>
+        <v>479</v>
       </c>
     </row>
     <row r="151" spans="1:4">
@@ -3571,13 +3925,13 @@
         <v>141</v>
       </c>
       <c r="B151" t="s">
-        <v>289</v>
+        <v>339</v>
       </c>
       <c r="C151" t="s">
-        <v>352</v>
+        <v>452</v>
       </c>
       <c r="D151" t="s">
-        <v>362</v>
+        <v>479</v>
       </c>
     </row>
     <row r="152" spans="1:4">
@@ -3585,13 +3939,13 @@
         <v>142</v>
       </c>
       <c r="B152" t="s">
-        <v>290</v>
+        <v>340</v>
       </c>
       <c r="C152" t="s">
-        <v>353</v>
+        <v>453</v>
       </c>
       <c r="D152" t="s">
-        <v>362</v>
+        <v>479</v>
       </c>
     </row>
     <row r="153" spans="1:4">
@@ -3599,13 +3953,13 @@
         <v>143</v>
       </c>
       <c r="B153" t="s">
-        <v>291</v>
+        <v>341</v>
       </c>
       <c r="C153" t="s">
-        <v>353</v>
+        <v>453</v>
       </c>
       <c r="D153" t="s">
-        <v>362</v>
+        <v>479</v>
       </c>
     </row>
     <row r="154" spans="1:4">
@@ -3613,13 +3967,13 @@
         <v>144</v>
       </c>
       <c r="B154" t="s">
-        <v>292</v>
+        <v>342</v>
       </c>
       <c r="C154" t="s">
-        <v>353</v>
+        <v>453</v>
       </c>
       <c r="D154" t="s">
-        <v>362</v>
+        <v>479</v>
       </c>
     </row>
     <row r="155" spans="1:4">
@@ -3627,13 +3981,13 @@
         <v>145</v>
       </c>
       <c r="B155" t="s">
-        <v>293</v>
+        <v>343</v>
       </c>
       <c r="C155" t="s">
-        <v>354</v>
+        <v>454</v>
       </c>
       <c r="D155" t="s">
-        <v>362</v>
+        <v>479</v>
       </c>
     </row>
     <row r="156" spans="1:4">
@@ -3641,13 +3995,13 @@
         <v>146</v>
       </c>
       <c r="B156" t="s">
-        <v>294</v>
+        <v>344</v>
       </c>
       <c r="C156" t="s">
-        <v>354</v>
+        <v>454</v>
       </c>
       <c r="D156" t="s">
-        <v>362</v>
+        <v>479</v>
       </c>
     </row>
     <row r="157" spans="1:4">
@@ -3655,13 +4009,13 @@
         <v>147</v>
       </c>
       <c r="B157" t="s">
-        <v>295</v>
+        <v>345</v>
       </c>
       <c r="C157" t="s">
-        <v>354</v>
+        <v>454</v>
       </c>
       <c r="D157" t="s">
-        <v>362</v>
+        <v>479</v>
       </c>
     </row>
     <row r="158" spans="1:4">
@@ -3669,13 +4023,13 @@
         <v>148</v>
       </c>
       <c r="B158" t="s">
-        <v>296</v>
+        <v>346</v>
       </c>
       <c r="C158" t="s">
-        <v>355</v>
+        <v>455</v>
       </c>
       <c r="D158" t="s">
-        <v>362</v>
+        <v>479</v>
       </c>
     </row>
     <row r="159" spans="1:4">
@@ -3683,13 +4037,13 @@
         <v>149</v>
       </c>
       <c r="B159" t="s">
-        <v>297</v>
+        <v>347</v>
       </c>
       <c r="C159" t="s">
-        <v>355</v>
+        <v>455</v>
       </c>
       <c r="D159" t="s">
-        <v>362</v>
+        <v>479</v>
       </c>
     </row>
     <row r="160" spans="1:4">
@@ -3697,13 +4051,13 @@
         <v>150</v>
       </c>
       <c r="B160" t="s">
-        <v>298</v>
+        <v>348</v>
       </c>
       <c r="C160" t="s">
-        <v>355</v>
+        <v>455</v>
       </c>
       <c r="D160" t="s">
-        <v>362</v>
+        <v>479</v>
       </c>
     </row>
     <row r="161" spans="1:4">
@@ -3711,24 +4065,724 @@
         <v>151</v>
       </c>
       <c r="B161" t="s">
-        <v>299</v>
+        <v>349</v>
       </c>
       <c r="C161" t="s">
-        <v>356</v>
+        <v>456</v>
       </c>
       <c r="D161" t="s">
-        <v>362</v>
+        <v>479</v>
       </c>
     </row>
     <row r="162" spans="1:4">
       <c r="B162" t="s">
-        <v>300</v>
+        <v>350</v>
       </c>
       <c r="C162" t="s">
+        <v>456</v>
+      </c>
+      <c r="D162" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="163" spans="1:4">
+      <c r="A163" t="s">
+        <v>152</v>
+      </c>
+      <c r="B163" t="s">
+        <v>351</v>
+      </c>
+      <c r="C163" t="s">
+        <v>457</v>
+      </c>
+      <c r="D163" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="164" spans="1:4">
+      <c r="A164" t="s">
+        <v>153</v>
+      </c>
+      <c r="B164" t="s">
+        <v>352</v>
+      </c>
+      <c r="C164" t="s">
+        <v>457</v>
+      </c>
+      <c r="D164" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="165" spans="1:4">
+      <c r="A165" t="s">
+        <v>154</v>
+      </c>
+      <c r="B165" t="s">
+        <v>353</v>
+      </c>
+      <c r="C165" t="s">
+        <v>457</v>
+      </c>
+      <c r="D165" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="166" spans="1:4">
+      <c r="A166" t="s">
+        <v>155</v>
+      </c>
+      <c r="B166" t="s">
+        <v>354</v>
+      </c>
+      <c r="C166" t="s">
+        <v>458</v>
+      </c>
+      <c r="D166" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="167" spans="1:4">
+      <c r="A167" t="s">
+        <v>156</v>
+      </c>
+      <c r="B167" t="s">
+        <v>355</v>
+      </c>
+      <c r="C167" t="s">
+        <v>458</v>
+      </c>
+      <c r="D167" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="168" spans="1:4">
+      <c r="A168" t="s">
+        <v>157</v>
+      </c>
+      <c r="B168" t="s">
         <v>356</v>
       </c>
-      <c r="D162" t="s">
+      <c r="C168" t="s">
+        <v>458</v>
+      </c>
+      <c r="D168" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="169" spans="1:4">
+      <c r="A169" t="s">
+        <v>158</v>
+      </c>
+      <c r="B169" t="s">
+        <v>357</v>
+      </c>
+      <c r="C169" t="s">
+        <v>459</v>
+      </c>
+      <c r="D169" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="170" spans="1:4">
+      <c r="A170" t="s">
+        <v>159</v>
+      </c>
+      <c r="B170" t="s">
+        <v>358</v>
+      </c>
+      <c r="C170" t="s">
+        <v>459</v>
+      </c>
+      <c r="D170" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="171" spans="1:4">
+      <c r="A171" t="s">
+        <v>160</v>
+      </c>
+      <c r="B171" t="s">
+        <v>359</v>
+      </c>
+      <c r="C171" t="s">
+        <v>459</v>
+      </c>
+      <c r="D171" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="172" spans="1:4">
+      <c r="A172" t="s">
+        <v>161</v>
+      </c>
+      <c r="B172" t="s">
+        <v>360</v>
+      </c>
+      <c r="C172" t="s">
+        <v>460</v>
+      </c>
+      <c r="D172" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="173" spans="1:4">
+      <c r="A173" t="s">
+        <v>162</v>
+      </c>
+      <c r="B173" t="s">
+        <v>361</v>
+      </c>
+      <c r="C173" t="s">
+        <v>460</v>
+      </c>
+      <c r="D173" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="174" spans="1:4">
+      <c r="A174" t="s">
+        <v>163</v>
+      </c>
+      <c r="B174" t="s">
         <v>362</v>
+      </c>
+      <c r="C174" t="s">
+        <v>460</v>
+      </c>
+      <c r="D174" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="175" spans="1:4">
+      <c r="A175" t="s">
+        <v>164</v>
+      </c>
+      <c r="B175" t="s">
+        <v>363</v>
+      </c>
+      <c r="C175" t="s">
+        <v>461</v>
+      </c>
+      <c r="D175" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="176" spans="1:4">
+      <c r="A176" t="s">
+        <v>165</v>
+      </c>
+      <c r="B176" t="s">
+        <v>364</v>
+      </c>
+      <c r="C176" t="s">
+        <v>461</v>
+      </c>
+      <c r="D176" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="177" spans="1:4">
+      <c r="A177" t="s">
+        <v>166</v>
+      </c>
+      <c r="B177" t="s">
+        <v>365</v>
+      </c>
+      <c r="C177" t="s">
+        <v>461</v>
+      </c>
+      <c r="D177" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="178" spans="1:4">
+      <c r="A178" t="s">
+        <v>167</v>
+      </c>
+      <c r="B178" t="s">
+        <v>366</v>
+      </c>
+      <c r="C178" t="s">
+        <v>462</v>
+      </c>
+      <c r="D178" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="179" spans="1:4">
+      <c r="A179" t="s">
+        <v>168</v>
+      </c>
+      <c r="B179" t="s">
+        <v>367</v>
+      </c>
+      <c r="C179" t="s">
+        <v>462</v>
+      </c>
+      <c r="D179" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="180" spans="1:4">
+      <c r="A180" t="s">
+        <v>169</v>
+      </c>
+      <c r="B180" t="s">
+        <v>368</v>
+      </c>
+      <c r="C180" t="s">
+        <v>463</v>
+      </c>
+      <c r="D180" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="181" spans="1:4">
+      <c r="A181" t="s">
+        <v>170</v>
+      </c>
+      <c r="B181" t="s">
+        <v>369</v>
+      </c>
+      <c r="C181" t="s">
+        <v>463</v>
+      </c>
+      <c r="D181" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="182" spans="1:4">
+      <c r="A182" t="s">
+        <v>171</v>
+      </c>
+      <c r="B182" t="s">
+        <v>370</v>
+      </c>
+      <c r="C182" t="s">
+        <v>463</v>
+      </c>
+      <c r="D182" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="183" spans="1:4">
+      <c r="A183" t="s">
+        <v>172</v>
+      </c>
+      <c r="B183" t="s">
+        <v>371</v>
+      </c>
+      <c r="C183" t="s">
+        <v>464</v>
+      </c>
+      <c r="D183" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="184" spans="1:4">
+      <c r="A184" t="s">
+        <v>173</v>
+      </c>
+      <c r="B184" t="s">
+        <v>372</v>
+      </c>
+      <c r="C184" t="s">
+        <v>464</v>
+      </c>
+      <c r="D184" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="185" spans="1:4">
+      <c r="A185" t="s">
+        <v>174</v>
+      </c>
+      <c r="B185" t="s">
+        <v>373</v>
+      </c>
+      <c r="C185" t="s">
+        <v>464</v>
+      </c>
+      <c r="D185" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="186" spans="1:4">
+      <c r="A186" t="s">
+        <v>175</v>
+      </c>
+      <c r="B186" t="s">
+        <v>374</v>
+      </c>
+      <c r="C186" t="s">
+        <v>465</v>
+      </c>
+      <c r="D186" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="187" spans="1:4">
+      <c r="A187" t="s">
+        <v>176</v>
+      </c>
+      <c r="B187" t="s">
+        <v>375</v>
+      </c>
+      <c r="C187" t="s">
+        <v>465</v>
+      </c>
+      <c r="D187" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="188" spans="1:4">
+      <c r="A188" t="s">
+        <v>177</v>
+      </c>
+      <c r="B188" t="s">
+        <v>376</v>
+      </c>
+      <c r="C188" t="s">
+        <v>465</v>
+      </c>
+      <c r="D188" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="189" spans="1:4">
+      <c r="A189" t="s">
+        <v>178</v>
+      </c>
+      <c r="B189" t="s">
+        <v>377</v>
+      </c>
+      <c r="C189" t="s">
+        <v>466</v>
+      </c>
+      <c r="D189" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="190" spans="1:4">
+      <c r="A190" t="s">
+        <v>179</v>
+      </c>
+      <c r="B190" t="s">
+        <v>378</v>
+      </c>
+      <c r="C190" t="s">
+        <v>466</v>
+      </c>
+      <c r="D190" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="191" spans="1:4">
+      <c r="A191" t="s">
+        <v>180</v>
+      </c>
+      <c r="B191" t="s">
+        <v>379</v>
+      </c>
+      <c r="C191" t="s">
+        <v>466</v>
+      </c>
+      <c r="D191" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="192" spans="1:4">
+      <c r="A192" t="s">
+        <v>181</v>
+      </c>
+      <c r="B192" t="s">
+        <v>380</v>
+      </c>
+      <c r="C192" t="s">
+        <v>467</v>
+      </c>
+      <c r="D192" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="193" spans="1:4">
+      <c r="A193" t="s">
+        <v>182</v>
+      </c>
+      <c r="B193" t="s">
+        <v>381</v>
+      </c>
+      <c r="C193" t="s">
+        <v>467</v>
+      </c>
+      <c r="D193" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="194" spans="1:4">
+      <c r="A194" t="s">
+        <v>183</v>
+      </c>
+      <c r="B194" t="s">
+        <v>382</v>
+      </c>
+      <c r="C194" t="s">
+        <v>467</v>
+      </c>
+      <c r="D194" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="195" spans="1:4">
+      <c r="A195" t="s">
+        <v>184</v>
+      </c>
+      <c r="B195" t="s">
+        <v>383</v>
+      </c>
+      <c r="C195" t="s">
+        <v>468</v>
+      </c>
+      <c r="D195" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="196" spans="1:4">
+      <c r="A196" t="s">
+        <v>185</v>
+      </c>
+      <c r="B196" t="s">
+        <v>384</v>
+      </c>
+      <c r="C196" t="s">
+        <v>468</v>
+      </c>
+      <c r="D196" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="197" spans="1:4">
+      <c r="A197" t="s">
+        <v>186</v>
+      </c>
+      <c r="B197" t="s">
+        <v>385</v>
+      </c>
+      <c r="C197" t="s">
+        <v>468</v>
+      </c>
+      <c r="D197" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="198" spans="1:4">
+      <c r="A198" t="s">
+        <v>187</v>
+      </c>
+      <c r="B198" t="s">
+        <v>386</v>
+      </c>
+      <c r="C198" t="s">
+        <v>469</v>
+      </c>
+      <c r="D198" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="199" spans="1:4">
+      <c r="A199" t="s">
+        <v>188</v>
+      </c>
+      <c r="B199" t="s">
+        <v>387</v>
+      </c>
+      <c r="C199" t="s">
+        <v>469</v>
+      </c>
+      <c r="D199" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="200" spans="1:4">
+      <c r="A200" t="s">
+        <v>189</v>
+      </c>
+      <c r="B200" t="s">
+        <v>388</v>
+      </c>
+      <c r="C200" t="s">
+        <v>469</v>
+      </c>
+      <c r="D200" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="201" spans="1:4">
+      <c r="A201" t="s">
+        <v>190</v>
+      </c>
+      <c r="B201" t="s">
+        <v>389</v>
+      </c>
+      <c r="C201" t="s">
+        <v>470</v>
+      </c>
+      <c r="D201" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="202" spans="1:4">
+      <c r="A202" t="s">
+        <v>191</v>
+      </c>
+      <c r="B202" t="s">
+        <v>390</v>
+      </c>
+      <c r="C202" t="s">
+        <v>470</v>
+      </c>
+      <c r="D202" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="203" spans="1:4">
+      <c r="A203" t="s">
+        <v>192</v>
+      </c>
+      <c r="B203" t="s">
+        <v>391</v>
+      </c>
+      <c r="C203" t="s">
+        <v>470</v>
+      </c>
+      <c r="D203" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="204" spans="1:4">
+      <c r="A204" t="s">
+        <v>193</v>
+      </c>
+      <c r="B204" t="s">
+        <v>392</v>
+      </c>
+      <c r="C204" t="s">
+        <v>471</v>
+      </c>
+      <c r="D204" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="205" spans="1:4">
+      <c r="A205" t="s">
+        <v>194</v>
+      </c>
+      <c r="B205" t="s">
+        <v>393</v>
+      </c>
+      <c r="C205" t="s">
+        <v>471</v>
+      </c>
+      <c r="D205" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="206" spans="1:4">
+      <c r="A206" t="s">
+        <v>195</v>
+      </c>
+      <c r="B206" t="s">
+        <v>394</v>
+      </c>
+      <c r="C206" t="s">
+        <v>471</v>
+      </c>
+      <c r="D206" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="207" spans="1:4">
+      <c r="A207" t="s">
+        <v>196</v>
+      </c>
+      <c r="B207" t="s">
+        <v>395</v>
+      </c>
+      <c r="C207" t="s">
+        <v>472</v>
+      </c>
+      <c r="D207" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="208" spans="1:4">
+      <c r="A208" t="s">
+        <v>197</v>
+      </c>
+      <c r="B208" t="s">
+        <v>396</v>
+      </c>
+      <c r="C208" t="s">
+        <v>472</v>
+      </c>
+      <c r="D208" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="209" spans="1:4">
+      <c r="A209" t="s">
+        <v>198</v>
+      </c>
+      <c r="B209" t="s">
+        <v>397</v>
+      </c>
+      <c r="C209" t="s">
+        <v>472</v>
+      </c>
+      <c r="D209" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="210" spans="1:4">
+      <c r="A210" t="s">
+        <v>199</v>
+      </c>
+      <c r="B210" t="s">
+        <v>398</v>
+      </c>
+      <c r="C210" t="s">
+        <v>473</v>
+      </c>
+      <c r="D210" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="211" spans="1:4">
+      <c r="A211" t="s">
+        <v>200</v>
+      </c>
+      <c r="B211" t="s">
+        <v>399</v>
+      </c>
+      <c r="C211" t="s">
+        <v>473</v>
+      </c>
+      <c r="D211" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="212" spans="1:4">
+      <c r="A212" t="s">
+        <v>201</v>
+      </c>
+      <c r="B212" t="s">
+        <v>400</v>
+      </c>
+      <c r="C212" t="s">
+        <v>473</v>
+      </c>
+      <c r="D212" t="s">
+        <v>480</v>
       </c>
     </row>
   </sheetData>

</xml_diff>